<commit_message>
Added in LDA test results
</commit_message>
<xml_diff>
--- a/TCR 2025 Results.xlsx
+++ b/TCR 2025 Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02fc7b328ab0cc43/Desktop/Github/TCR-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B25845F4-E042-4637-B5C4-81628C66F10C}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FCB5E9C-0265-4876-B0B4-48FC4358E086}"/>
   <bookViews>
     <workbookView xWindow="47895" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>Method</t>
   </si>
@@ -91,13 +91,16 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>LDA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +127,14 @@
       <b/>
       <sz val="12"/>
       <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -155,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -166,11 +177,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -497,7 +511,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,11 +540,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
         <v>45949</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -543,7 +557,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
         <v>7</v>
@@ -551,11 +565,11 @@
       <c r="D3" s="2">
         <v>0.72729999999999995</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -567,7 +581,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
         <v>9</v>
@@ -577,7 +591,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:8" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
         <v>10</v>
@@ -587,7 +601,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:8" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
         <v>11</v>
@@ -597,7 +611,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:8" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>12</v>
@@ -607,7 +621,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:8" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
         <v>13</v>
@@ -618,10 +632,10 @@
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="6">
         <v>45949</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -631,12 +645,12 @@
         <v>0.68179999999999996</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
+      <c r="A11" s="4"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
         <v>7</v>
@@ -645,12 +659,12 @@
         <v>0.72729999999999995</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
+      <c r="A12" s="4"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
         <v>8</v>
@@ -659,12 +673,12 @@
         <v>0.72729999999999995</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+      <c r="A13" s="4"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
         <v>9</v>
@@ -673,12 +687,12 @@
         <v>0.72729999999999995</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
+      <c r="A14" s="4"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
         <v>10</v>
@@ -687,227 +701,263 @@
         <v>0.63639999999999997</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
+      <c r="A15" s="4"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
+      <c r="A16" s="4"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
+      <c r="A17" s="4"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="A18" s="6">
+        <v>45949</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.68179999999999996</v>
+      </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
+      <c r="A19" s="4"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.77270000000000005</v>
+      </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
+      <c r="A20" s="4"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.77270000000000005</v>
+      </c>
       <c r="E20" s="2"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
+      <c r="A21" s="4"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.77270000000000005</v>
+      </c>
       <c r="E21" s="2"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
+      <c r="A22" s="4"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.81820000000000004</v>
+      </c>
       <c r="E22" s="2"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
+      <c r="A23" s="4"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="C23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.77270000000000005</v>
+      </c>
       <c r="E23" s="2"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
+      <c r="A24" s="4"/>
       <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.77270000000000005</v>
+      </c>
       <c r="E24" s="2"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
+      <c r="A25" s="4"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.72729999999999995</v>
+      </c>
       <c r="E25" s="2"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
+      <c r="A26" s="4"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
+      <c r="A27" s="4"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
+      <c r="A28" s="4"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
+      <c r="A29" s="4"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
+      <c r="A30" s="4"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
+      <c r="A31" s="4"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
     </row>
     <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
+      <c r="A32" s="4"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
     </row>
     <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
+      <c r="A33" s="4"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
     </row>
     <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
+      <c r="A34" s="4"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added KNN k=3 results
</commit_message>
<xml_diff>
--- a/TCR 2025 Results.xlsx
+++ b/TCR 2025 Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02fc7b328ab0cc43/Desktop/Github/TCR-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FCB5E9C-0265-4876-B0B4-48FC4358E086}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C014C99-B69C-4D17-A7BB-B669FC4FCB7A}"/>
   <bookViews>
     <workbookView xWindow="47895" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="27">
   <si>
     <t>Method</t>
   </si>
@@ -94,6 +94,31 @@
   </si>
   <si>
     <t>LDA</t>
+  </si>
+  <si>
+    <t>KNN</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k=3</t>
+    </r>
+  </si>
+  <si>
+    <t>k=5</t>
+  </si>
+  <si>
+    <t>k=7</t>
   </si>
 </sst>
 </file>
@@ -140,7 +165,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -150,6 +175,42 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB7ADF5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF669900"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33CCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0099FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6699FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -166,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -184,7 +245,25 @@
     <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -195,6 +274,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF6699FF"/>
+      <color rgb="FF0099FF"/>
+      <color rgb="FF33CCCC"/>
+      <color rgb="FFFF6600"/>
+      <color rgb="FF669900"/>
       <color rgb="FFE20000"/>
       <color rgb="FFB7ADF5"/>
       <color rgb="FFCC66FF"/>
@@ -508,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F10ACA-FE60-4476-A75C-BE5F9F7050CA}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,7 +719,7 @@
       <c r="A10" s="6">
         <v>45949</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -757,7 +841,7 @@
       <c r="A18" s="6">
         <v>45949</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -870,10 +954,18 @@
       <c r="H25" s="4"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+      <c r="A26" s="6">
+        <v>45949</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.72729999999999995</v>
+      </c>
       <c r="E26" s="2"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -881,9 +973,15 @@
     </row>
     <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="B27" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.72729999999999995</v>
+      </c>
       <c r="E27" s="2"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
@@ -892,8 +990,12 @@
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.81820000000000004</v>
+      </c>
       <c r="E28" s="2"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -902,8 +1004,12 @@
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.77270000000000005</v>
+      </c>
       <c r="E29" s="2"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
@@ -912,8 +1018,12 @@
     <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.81820000000000004</v>
+      </c>
       <c r="E30" s="2"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
@@ -922,8 +1032,12 @@
     <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+      <c r="C31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.77270000000000005</v>
+      </c>
       <c r="E31" s="2"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -932,8 +1046,12 @@
     <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="C32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.81820000000000004</v>
+      </c>
       <c r="E32" s="2"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
@@ -942,23 +1060,146 @@
     <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
+      <c r="C33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.72729999999999995</v>
+      </c>
       <c r="E33" s="2"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
     </row>
     <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
+      <c r="A34" s="6">
+        <v>45949</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
     </row>
+    <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
+        <v>45949</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added KNN k=5 results
</commit_message>
<xml_diff>
--- a/TCR 2025 Results.xlsx
+++ b/TCR 2025 Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02fc7b328ab0cc43/Desktop/Github/TCR-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C014C99-B69C-4D17-A7BB-B669FC4FCB7A}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E9FFCCD-A258-438D-AEEC-3E9852BF3325}"/>
   <bookViews>
     <workbookView xWindow="47895" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
   </bookViews>
@@ -594,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F10ACA-FE60-4476-A75C-BE5F9F7050CA}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,7 +1081,9 @@
       <c r="C34" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="2"/>
+      <c r="D34" s="2">
+        <v>0.72729999999999995</v>
+      </c>
       <c r="E34" s="2"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
@@ -1094,6 +1096,9 @@
       </c>
       <c r="C35" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.77270000000000005</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1102,6 +1107,9 @@
       <c r="C36" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="D36" s="2">
+        <v>0.77270000000000005</v>
+      </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
@@ -1109,6 +1117,9 @@
       <c r="C37" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D37" s="2">
+        <v>0.77270000000000005</v>
+      </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
@@ -1116,6 +1127,9 @@
       <c r="C38" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D38" s="2">
+        <v>0.77270000000000005</v>
+      </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
@@ -1123,6 +1137,9 @@
       <c r="C39" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D39" s="2">
+        <v>0.77270000000000005</v>
+      </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
@@ -1130,6 +1147,9 @@
       <c r="C40" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D40" s="2">
+        <v>0.77270000000000005</v>
+      </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
@@ -1137,6 +1157,9 @@
       <c r="C41" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D41" s="2">
+        <v>0.77270000000000005</v>
+      </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="6">

</xml_diff>

<commit_message>
Added KNN k=7 results
</commit_message>
<xml_diff>
--- a/TCR 2025 Results.xlsx
+++ b/TCR 2025 Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02fc7b328ab0cc43/Desktop/Github/TCR-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E9FFCCD-A258-438D-AEEC-3E9852BF3325}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B47306F7-5053-4888-9165-5EEB354D9209}"/>
   <bookViews>
     <workbookView xWindow="47895" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
   </bookViews>
@@ -595,7 +595,7 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,6 +1171,9 @@
       <c r="C42" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="D42" s="2">
+        <v>0.72729999999999995</v>
+      </c>
     </row>
     <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
@@ -1179,6 +1182,9 @@
       </c>
       <c r="C43" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.77270000000000005</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1187,6 +1193,9 @@
       <c r="C44" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="D44" s="2">
+        <v>0.77270000000000005</v>
+      </c>
     </row>
     <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
@@ -1194,6 +1203,9 @@
       <c r="C45" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D45" s="2">
+        <v>0.72729999999999995</v>
+      </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
@@ -1201,6 +1213,9 @@
       <c r="C46" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D46" s="2">
+        <v>0.72729999999999995</v>
+      </c>
     </row>
     <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
@@ -1208,6 +1223,9 @@
       <c r="C47" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D47" s="2">
+        <v>0.81820000000000004</v>
+      </c>
     </row>
     <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
@@ -1215,12 +1233,18 @@
       <c r="C48" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D48" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.86360000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added regression tree, bagging, random forest, boosting slots
</commit_message>
<xml_diff>
--- a/TCR 2025 Results.xlsx
+++ b/TCR 2025 Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02fc7b328ab0cc43/Desktop/Github/TCR-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B47306F7-5053-4888-9165-5EEB354D9209}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98FDDF53-4509-47EF-8015-C2DBACB19672}"/>
   <bookViews>
-    <workbookView xWindow="47895" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
+    <workbookView xWindow="34125" yWindow="600" windowWidth="27630" windowHeight="14880" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="34">
   <si>
     <t>Method</t>
   </si>
@@ -119,6 +119,27 @@
   </si>
   <si>
     <t>k=7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regression </t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
+    <t>Test Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bagging </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Random </t>
+  </si>
+  <si>
+    <t>Forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boosting </t>
   </si>
 </sst>
 </file>
@@ -165,7 +186,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,6 +235,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE20000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD21C1C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE21498"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -227,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -264,6 +309,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -274,13 +334,15 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE20000"/>
+      <color rgb="FFE21498"/>
+      <color rgb="FFD21C1C"/>
+      <color rgb="FFB7ADF5"/>
       <color rgb="FF6699FF"/>
       <color rgb="FF0099FF"/>
       <color rgb="FF33CCCC"/>
       <color rgb="FFFF6600"/>
       <color rgb="FF669900"/>
-      <color rgb="FFE20000"/>
-      <color rgb="FFB7ADF5"/>
       <color rgb="FFCC66FF"/>
     </mruColors>
   </colors>
@@ -592,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F10ACA-FE60-4476-A75C-BE5F9F7050CA}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,7 +1299,7 @@
         <v>0.81820000000000004</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
@@ -1245,6 +1307,243 @@
       </c>
       <c r="D49" s="2">
         <v>0.86360000000000003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A50" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="6"/>
+      <c r="B51" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" s="2"/>
+    </row>
+    <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B59" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B60" s="15"/>
+      <c r="C60" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B61" s="2"/>
+      <c r="C61" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B62" s="2"/>
+      <c r="C62" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B63" s="2"/>
+      <c r="C63" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B64" s="2"/>
+      <c r="C64" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B65" s="2"/>
+      <c r="C65" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B66" s="2"/>
+      <c r="C66" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B67" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B68" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B69" s="2"/>
+      <c r="C69" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B70" s="2"/>
+      <c r="C70" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B71" s="2"/>
+      <c r="C71" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B72" s="2"/>
+      <c r="C72" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B73" s="2"/>
+      <c r="C73" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B74" s="2"/>
+      <c r="C74" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B75" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B76" s="15"/>
+      <c r="C76" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B77" s="2"/>
+      <c r="C77" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B78" s="2"/>
+      <c r="C78" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B79" s="2"/>
+      <c r="C79" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B80" s="2"/>
+      <c r="C80" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B81" s="2"/>
+      <c r="C81" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B82" s="2"/>
+      <c r="C82" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made a Ranking sheet in Results
</commit_message>
<xml_diff>
--- a/TCR 2025 Results.xlsx
+++ b/TCR 2025 Results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02fc7b328ab0cc43/Desktop/Github/TCR-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98FDDF53-4509-47EF-8015-C2DBACB19672}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C3BE561-1211-4BE4-B9A7-6B09DD356BDA}"/>
   <bookViews>
-    <workbookView xWindow="34125" yWindow="600" windowWidth="27630" windowHeight="14880" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
+    <workbookView xWindow="33405" yWindow="600" windowWidth="27630" windowHeight="14880" activeTab="1" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Record" sheetId="1" r:id="rId1"/>
+    <sheet name="Ranking" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="44">
   <si>
     <t>Method</t>
   </si>
@@ -121,9 +122,6 @@
     <t>k=7</t>
   </si>
   <si>
-    <t xml:space="preserve">Regression </t>
-  </si>
-  <si>
     <t>Tree</t>
   </si>
   <si>
@@ -140,6 +138,39 @@
   </si>
   <si>
     <t xml:space="preserve">Boosting </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classification </t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Best Method</t>
+  </si>
+  <si>
+    <t>Highest Val</t>
+  </si>
+  <si>
+    <t>KNN: k=7</t>
+  </si>
+  <si>
+    <t>Most incomplete</t>
+  </si>
+  <si>
+    <t>KNN: k=3</t>
+  </si>
+  <si>
+    <t>Group(s)</t>
+  </si>
+  <si>
+    <t>Top 15, 25,35</t>
+  </si>
+  <si>
+    <t>KNN: k=5</t>
+  </si>
+  <si>
+    <t>Top 10-37</t>
   </si>
 </sst>
 </file>
@@ -186,7 +217,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -237,12 +268,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE20000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFD21C1C"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -255,7 +280,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -272,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -311,19 +336,16 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -656,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F10ACA-FE60-4476-A75C-BE5F9F7050CA}">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1320,7 +1342,7 @@
         <v>1</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>3</v>
@@ -1328,8 +1350,8 @@
     </row>
     <row r="51" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
-      <c r="B51" s="17" t="s">
-        <v>27</v>
+      <c r="B51" s="16" t="s">
+        <v>33</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>6</v>
@@ -1338,8 +1360,8 @@
     </row>
     <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
-      <c r="B52" s="17" t="s">
-        <v>28</v>
+      <c r="B52" s="16" t="s">
+        <v>27</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>7</v>
@@ -1395,15 +1417,15 @@
       <c r="D58" s="2"/>
     </row>
     <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B59" s="16" t="s">
-        <v>30</v>
+      <c r="B59" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B60" s="15"/>
+      <c r="B60" s="14"/>
       <c r="C60" s="2" t="s">
         <v>7</v>
       </c>
@@ -1445,16 +1467,16 @@
       </c>
     </row>
     <row r="67" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B67" s="14" t="s">
-        <v>31</v>
+      <c r="B67" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="68" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B68" s="14" t="s">
-        <v>32</v>
+      <c r="B68" s="17" t="s">
+        <v>31</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>7</v>
@@ -1497,15 +1519,15 @@
       </c>
     </row>
     <row r="75" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B75" s="18" t="s">
-        <v>33</v>
+      <c r="B75" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="76" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B76" s="15"/>
+      <c r="B76" s="14"/>
       <c r="C76" s="2" t="s">
         <v>7</v>
       </c>
@@ -1550,4 +1572,1119 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D437B6-726D-4DC3-85CA-C3D4328315ED}">
+  <dimension ref="A1:J82"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="19.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="24.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.86360000000000003</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2">
+        <v>3</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2">
+        <v>4</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2">
+        <v>6</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="2">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.63639999999999997</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="2">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="2">
+        <v>7</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="2">
+        <v>8</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="2">
+        <v>3</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="2">
+        <v>4</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="2">
+        <v>5</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>6</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2">
+        <v>7</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="2">
+        <v>8</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="2">
+        <v>3</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="2">
+        <v>4</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="2">
+        <v>5</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="2">
+        <v>6</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="2">
+        <v>7</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="2">
+        <v>8</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="2">
+        <v>2</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="2">
+        <v>3</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="2">
+        <v>4</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="2">
+        <v>5</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="2">
+        <v>6</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="2">
+        <v>7</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" s="2">
+        <v>8</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="2">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.86360000000000003</v>
+      </c>
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" s="2">
+        <v>2</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="2">
+        <v>3</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="2">
+        <v>4</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="2">
+        <v>5</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="2">
+        <v>6</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="2">
+        <v>7</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" s="2">
+        <v>8</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="1:5" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.35"/>
+    <row r="51" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B51" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B52" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B53" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B55" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B57" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B58" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B59" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B60" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B61" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B62" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B63" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B64" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B65" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B66" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B67" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B68" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B69" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B70" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B71" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B72" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B73" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B74" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B75" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B76" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B77" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B78" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B79" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B80" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B81" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B82" s="2">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated results and ranking sheet
</commit_message>
<xml_diff>
--- a/TCR 2025 Results.xlsx
+++ b/TCR 2025 Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02fc7b328ab0cc43/Desktop/Github/TCR-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C3BE561-1211-4BE4-B9A7-6B09DD356BDA}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCA73AD4-65A6-4904-9D35-B6662227ADA2}"/>
   <bookViews>
-    <workbookView xWindow="33405" yWindow="600" windowWidth="27630" windowHeight="14880" activeTab="1" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
+    <workbookView xWindow="47895" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="1" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Record" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="44">
   <si>
     <t>Method</t>
   </si>
@@ -297,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -347,6 +347,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -678,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F10ACA-FE60-4476-A75C-BE5F9F7050CA}">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51:D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,14 +1352,18 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
+      <c r="A51" s="6">
+        <v>45952</v>
+      </c>
       <c r="B51" s="16" t="s">
         <v>33</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D51" s="2"/>
+      <c r="D51" s="18">
+        <v>0.40910000000000002</v>
+      </c>
     </row>
     <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
@@ -1366,7 +1373,9 @@
       <c r="C52" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D52" s="2"/>
+      <c r="D52" s="2">
+        <v>0.31819999999999998</v>
+      </c>
     </row>
     <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
@@ -1374,7 +1383,9 @@
       <c r="C53" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D53" s="2"/>
+      <c r="D53" s="2">
+        <v>0.31819999999999998</v>
+      </c>
     </row>
     <row r="54" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
@@ -1382,7 +1393,9 @@
       <c r="C54" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D54" s="2"/>
+      <c r="D54" s="2">
+        <v>0.2727</v>
+      </c>
     </row>
     <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
@@ -1390,7 +1403,9 @@
       <c r="C55" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D55" s="2"/>
+      <c r="D55" s="2">
+        <v>0.2727</v>
+      </c>
     </row>
     <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
@@ -1398,7 +1413,9 @@
       <c r="C56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D56" s="2"/>
+      <c r="D56" s="2">
+        <v>0.36359999999999998</v>
+      </c>
     </row>
     <row r="57" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
@@ -1406,7 +1423,9 @@
       <c r="C57" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D57" s="2"/>
+      <c r="D57" s="2">
+        <v>0.31819999999999998</v>
+      </c>
     </row>
     <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
@@ -1414,7 +1433,9 @@
       <c r="C58" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D58" s="2"/>
+      <c r="D58" s="2">
+        <v>0.31819999999999998</v>
+      </c>
     </row>
     <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="15" t="s">
@@ -1579,7 +1600,7 @@
   <dimension ref="A1:J82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="C56" sqref="C56:D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2435,6 +2456,12 @@
       <c r="B51" s="2">
         <v>1</v>
       </c>
+      <c r="C51" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0.2727</v>
+      </c>
     </row>
     <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
@@ -2443,6 +2470,12 @@
       <c r="B52" s="2">
         <v>2</v>
       </c>
+      <c r="C52" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" s="2">
+        <v>0.2727</v>
+      </c>
     </row>
     <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
@@ -2451,6 +2484,12 @@
       <c r="B53" s="2">
         <v>3</v>
       </c>
+      <c r="C53" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0.36359999999999998</v>
+      </c>
     </row>
     <row r="54" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
@@ -2459,6 +2498,12 @@
       <c r="B54" s="2">
         <v>4</v>
       </c>
+      <c r="C54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="2">
+        <v>0.31819999999999998</v>
+      </c>
     </row>
     <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
@@ -2467,6 +2512,12 @@
       <c r="B55" s="2">
         <v>5</v>
       </c>
+      <c r="C55" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" s="2">
+        <v>0.31819999999999998</v>
+      </c>
     </row>
     <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
@@ -2475,6 +2526,12 @@
       <c r="B56" s="2">
         <v>6</v>
       </c>
+      <c r="C56" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0.31819999999999998</v>
+      </c>
     </row>
     <row r="57" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
@@ -2483,6 +2540,12 @@
       <c r="B57" s="2">
         <v>7</v>
       </c>
+      <c r="C57" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0.31819999999999998</v>
+      </c>
     </row>
     <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="16" t="s">
@@ -2490,6 +2553,12 @@
       </c>
       <c r="B58" s="2">
         <v>8</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="18">
+        <v>0.40910000000000002</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added bagging results to record and rank sheets
</commit_message>
<xml_diff>
--- a/TCR 2025 Results.xlsx
+++ b/TCR 2025 Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02fc7b328ab0cc43/Desktop/Github/TCR-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCA73AD4-65A6-4904-9D35-B6662227ADA2}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33221FAF-06B5-4CD4-B39D-80661676F8E0}"/>
   <bookViews>
-    <workbookView xWindow="47895" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="1" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
+    <workbookView xWindow="39570" yWindow="495" windowWidth="27630" windowHeight="14880" activeTab="1" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Record" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="44">
   <si>
     <t>Method</t>
   </si>
@@ -681,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F10ACA-FE60-4476-A75C-BE5F9F7050CA}">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51:D58"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59:D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,150 +1444,190 @@
       <c r="C59" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="D59" s="2">
+        <v>0.2727</v>
+      </c>
     </row>
     <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="14"/>
       <c r="C60" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="D60" s="2">
+        <v>0.2273</v>
+      </c>
     </row>
     <row r="61" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
       <c r="C61" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="D61" s="2">
+        <v>0.2273</v>
+      </c>
     </row>
     <row r="62" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
       <c r="C62" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D62" s="2">
+        <v>0.2727</v>
+      </c>
     </row>
     <row r="63" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
       <c r="C63" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D63" s="2">
+        <v>0.2273</v>
+      </c>
     </row>
     <row r="64" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
       <c r="C64" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="65" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D64" s="2">
+        <v>0.2273</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
       <c r="C65" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="66" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D65" s="2">
+        <v>0.18179999999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
       <c r="C66" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="67" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D66" s="2">
+        <v>0.2727</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B67" s="17" t="s">
         <v>30</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="68" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B68" s="17" t="s">
         <v>31</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="69" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B69" s="2"/>
       <c r="C69" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="70" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B70" s="2"/>
       <c r="C70" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="71" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B71" s="2"/>
       <c r="C71" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="72" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="73" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B73" s="2"/>
       <c r="C73" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="74" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="75" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B75" s="9" t="s">
         <v>32</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="76" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B76" s="14"/>
       <c r="C76" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="77" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B77" s="2"/>
       <c r="C77" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="78" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B78" s="2"/>
       <c r="C78" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="79" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B79" s="2"/>
       <c r="C79" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="80" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B80" s="2"/>
       <c r="C80" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="81" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B81" s="2"/>
       <c r="C81" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="82" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B82" s="2"/>
       <c r="C82" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D82" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1599,8 +1639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D437B6-726D-4DC3-85CA-C3D4328315ED}">
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56:D57"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60:D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2568,6 +2608,12 @@
       <c r="B59" s="2">
         <v>1</v>
       </c>
+      <c r="C59" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" s="2">
+        <v>0.18179999999999999</v>
+      </c>
     </row>
     <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="15" t="s">
@@ -2576,6 +2622,12 @@
       <c r="B60" s="2">
         <v>2</v>
       </c>
+      <c r="C60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="2">
+        <v>0.2273</v>
+      </c>
     </row>
     <row r="61" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
@@ -2584,6 +2636,12 @@
       <c r="B61" s="2">
         <v>3</v>
       </c>
+      <c r="C61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" s="2">
+        <v>0.2273</v>
+      </c>
     </row>
     <row r="62" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
@@ -2592,6 +2650,12 @@
       <c r="B62" s="2">
         <v>4</v>
       </c>
+      <c r="C62" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" s="2">
+        <v>0.2273</v>
+      </c>
     </row>
     <row r="63" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="15" t="s">
@@ -2600,6 +2664,12 @@
       <c r="B63" s="2">
         <v>5</v>
       </c>
+      <c r="C63" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D63" s="2">
+        <v>0.2273</v>
+      </c>
     </row>
     <row r="64" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="15" t="s">
@@ -2608,24 +2678,42 @@
       <c r="B64" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" s="2">
+        <v>0.2727</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="15" t="s">
         <v>29</v>
       </c>
       <c r="B65" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C65" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D65" s="2">
+        <v>0.2727</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
         <v>29</v>
       </c>
       <c r="B66" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C66" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D66" s="2">
+        <v>0.2727</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="17" t="s">
         <v>30</v>
       </c>
@@ -2633,7 +2721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
         <v>31</v>
       </c>
@@ -2641,7 +2729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="17" t="s">
         <v>30</v>
       </c>
@@ -2649,7 +2737,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="17" t="s">
         <v>31</v>
       </c>
@@ -2657,7 +2745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="17" t="s">
         <v>30</v>
       </c>
@@ -2665,7 +2753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="17" t="s">
         <v>31</v>
       </c>
@@ -2673,7 +2761,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="17" t="s">
         <v>30</v>
       </c>
@@ -2681,7 +2769,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="17" t="s">
         <v>31</v>
       </c>
@@ -2689,7 +2777,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>32</v>
       </c>
@@ -2697,7 +2785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>32</v>
       </c>
@@ -2705,7 +2793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>32</v>
       </c>
@@ -2713,7 +2801,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>32</v>
       </c>
@@ -2721,7 +2809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>32</v>
       </c>
@@ -2729,7 +2817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Added bagging results 2nd run to record and ranks sheets
</commit_message>
<xml_diff>
--- a/TCR 2025 Results.xlsx
+++ b/TCR 2025 Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02fc7b328ab0cc43/Desktop/Github/TCR-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33221FAF-06B5-4CD4-B39D-80661676F8E0}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C81AA1E-13FD-490B-B37E-33D68D79E9CA}"/>
   <bookViews>
     <workbookView xWindow="39570" yWindow="495" windowWidth="27630" windowHeight="14880" activeTab="1" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="48">
   <si>
     <t>Method</t>
   </si>
@@ -171,6 +171,18 @@
   </si>
   <si>
     <t>Top 10-37</t>
+  </si>
+  <si>
+    <t>1st run</t>
+  </si>
+  <si>
+    <t>2nd run</t>
+  </si>
+  <si>
+    <t>Bagging V1</t>
+  </si>
+  <si>
+    <t>Bagging V2</t>
   </si>
 </sst>
 </file>
@@ -217,7 +229,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,6 +296,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE82A0A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -297,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -351,6 +369,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -359,6 +380,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE82A0A"/>
       <color rgb="FFE20000"/>
       <color rgb="FFE21498"/>
       <color rgb="FFD21C1C"/>
@@ -368,7 +390,6 @@
       <color rgb="FF33CCCC"/>
       <color rgb="FFFF6600"/>
       <color rgb="FF669900"/>
-      <color rgb="FFCC66FF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -679,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F10ACA-FE60-4476-A75C-BE5F9F7050CA}">
-  <dimension ref="A1:H82"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59:D66"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67:D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1438,6 +1459,9 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
+        <v>45952</v>
+      </c>
       <c r="B59" s="15" t="s">
         <v>29</v>
       </c>
@@ -1448,7 +1472,10 @@
         <v>0.2727</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="B60" s="14"/>
       <c r="C60" s="2" t="s">
         <v>7</v>
@@ -1493,7 +1520,7 @@
         <v>0.2273</v>
       </c>
     </row>
-    <row r="65" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
       <c r="C65" s="2" t="s">
         <v>12</v>
@@ -1502,7 +1529,7 @@
         <v>0.18179999999999999</v>
       </c>
     </row>
-    <row r="66" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
       <c r="C66" s="2" t="s">
         <v>13</v>
@@ -1511,104 +1538,124 @@
         <v>0.2727</v>
       </c>
     </row>
-    <row r="67" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B67" s="17" t="s">
-        <v>30</v>
-      </c>
+    <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="6">
+        <v>45952</v>
+      </c>
+      <c r="B67" s="2"/>
       <c r="C67" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D67" s="2"/>
-    </row>
-    <row r="68" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B68" s="17" t="s">
-        <v>31</v>
-      </c>
+      <c r="D67" s="2">
+        <v>0.2273</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B68" s="2"/>
       <c r="C68" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D68" s="2"/>
-    </row>
-    <row r="69" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D68" s="2">
+        <v>0.2273</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B69" s="2"/>
       <c r="C69" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D69" s="2"/>
-    </row>
-    <row r="70" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D69" s="2">
+        <v>0.18179999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B70" s="2"/>
       <c r="C70" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D70" s="2"/>
-    </row>
-    <row r="71" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D70" s="2">
+        <v>0.2727</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B71" s="2"/>
       <c r="C71" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D71" s="2"/>
-    </row>
-    <row r="72" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D71" s="2">
+        <v>0.2727</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D72" s="2"/>
-    </row>
-    <row r="73" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D72" s="2">
+        <v>0.18179999999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B73" s="2"/>
       <c r="C73" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D73" s="2"/>
-    </row>
-    <row r="74" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D73" s="2">
+        <v>0.18179999999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D74" s="2"/>
-    </row>
-    <row r="75" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B75" s="9" t="s">
-        <v>32</v>
+      <c r="D74" s="2">
+        <v>0.2727</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B75" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B76" s="14"/>
+    <row r="76" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B76" s="17" t="s">
+        <v>31</v>
+      </c>
       <c r="C76" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B77" s="2"/>
       <c r="C77" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B78" s="2"/>
       <c r="C78" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B79" s="2"/>
       <c r="C79" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B80" s="2"/>
       <c r="C80" s="2" t="s">
         <v>11</v>
@@ -1628,6 +1675,64 @@
         <v>13</v>
       </c>
       <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B83" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B84" s="14"/>
+      <c r="C84" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D84" s="2"/>
+    </row>
+    <row r="85" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B85" s="2"/>
+      <c r="C85" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" s="2"/>
+    </row>
+    <row r="86" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B86" s="2"/>
+      <c r="C86" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D86" s="2"/>
+    </row>
+    <row r="87" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B87" s="2"/>
+      <c r="C87" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D87" s="2"/>
+    </row>
+    <row r="88" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B88" s="2"/>
+      <c r="C88" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B89" s="2"/>
+      <c r="C89" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D89" s="2"/>
+    </row>
+    <row r="90" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B90" s="2"/>
+      <c r="C90" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D90" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1637,10 +1742,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D437B6-726D-4DC3-85CA-C3D4328315ED}">
-  <dimension ref="A1:J82"/>
+  <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60:D61"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2603,7 +2708,7 @@
     </row>
     <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B59" s="2">
         <v>1</v>
@@ -2617,7 +2722,7 @@
     </row>
     <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="15" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B60" s="2">
         <v>2</v>
@@ -2631,7 +2736,7 @@
     </row>
     <row r="61" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B61" s="2">
         <v>3</v>
@@ -2645,7 +2750,7 @@
     </row>
     <row r="62" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B62" s="2">
         <v>4</v>
@@ -2659,7 +2764,7 @@
     </row>
     <row r="63" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="15" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B63" s="2">
         <v>5</v>
@@ -2673,7 +2778,7 @@
     </row>
     <row r="64" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="15" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B64" s="2">
         <v>6</v>
@@ -2687,7 +2792,7 @@
     </row>
     <row r="65" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="15" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B65" s="2">
         <v>7</v>
@@ -2701,7 +2806,7 @@
     </row>
     <row r="66" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B66" s="2">
         <v>8</v>
@@ -2714,130 +2819,242 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="17" t="s">
-        <v>30</v>
+      <c r="A67" s="19" t="s">
+        <v>47</v>
       </c>
       <c r="B67" s="2">
         <v>1</v>
       </c>
+      <c r="C67" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" s="2">
+        <v>0.18179999999999999</v>
+      </c>
     </row>
     <row r="68" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="17" t="s">
-        <v>31</v>
+      <c r="A68" s="19" t="s">
+        <v>47</v>
       </c>
       <c r="B68" s="2">
         <v>2</v>
       </c>
+      <c r="C68" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D68" s="2">
+        <v>0.18179999999999999</v>
+      </c>
     </row>
     <row r="69" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="17" t="s">
-        <v>30</v>
+      <c r="A69" s="19" t="s">
+        <v>47</v>
       </c>
       <c r="B69" s="2">
         <v>3</v>
       </c>
+      <c r="C69" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" s="2">
+        <v>0.18179999999999999</v>
+      </c>
     </row>
     <row r="70" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="17" t="s">
-        <v>31</v>
+      <c r="A70" s="19" t="s">
+        <v>47</v>
       </c>
       <c r="B70" s="2">
         <v>4</v>
       </c>
+      <c r="C70" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" s="2">
+        <v>0.2273</v>
+      </c>
     </row>
     <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="17" t="s">
-        <v>30</v>
+      <c r="A71" s="19" t="s">
+        <v>47</v>
       </c>
       <c r="B71" s="2">
         <v>5</v>
       </c>
+      <c r="C71" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" s="2">
+        <v>0.2273</v>
+      </c>
     </row>
     <row r="72" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="17" t="s">
-        <v>31</v>
+      <c r="A72" s="19" t="s">
+        <v>47</v>
       </c>
       <c r="B72" s="2">
         <v>6</v>
       </c>
+      <c r="C72" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D72" s="2">
+        <v>0.2727</v>
+      </c>
     </row>
     <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="17" t="s">
-        <v>30</v>
+      <c r="A73" s="19" t="s">
+        <v>47</v>
       </c>
       <c r="B73" s="2">
         <v>7</v>
       </c>
+      <c r="C73" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D73" s="2">
+        <v>0.2727</v>
+      </c>
     </row>
     <row r="74" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="17" t="s">
-        <v>31</v>
+      <c r="A74" s="19" t="s">
+        <v>47</v>
       </c>
       <c r="B74" s="2">
         <v>8</v>
       </c>
+      <c r="C74" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D74" s="2">
+        <v>0.2727</v>
+      </c>
     </row>
     <row r="75" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="9" t="s">
-        <v>32</v>
+      <c r="A75" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="B75" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="9" t="s">
-        <v>32</v>
+      <c r="A76" s="17" t="s">
+        <v>31</v>
       </c>
       <c r="B76" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="9" t="s">
-        <v>32</v>
+      <c r="A77" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="B77" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="9" t="s">
-        <v>32</v>
+      <c r="A78" s="17" t="s">
+        <v>31</v>
       </c>
       <c r="B78" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="9" t="s">
-        <v>32</v>
+      <c r="A79" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="B79" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="9" t="s">
+      <c r="A80" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B80" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B81" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B82" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A83" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B80" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A81" s="9" t="s">
+      <c r="B83" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B81" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A82" s="9" t="s">
+      <c r="B84" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B85" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B86" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B87" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B88" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A89" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B89" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A90" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B90" s="2">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Put in some notes for the warnings, need to make test error into accuracy now for consistency
</commit_message>
<xml_diff>
--- a/TCR 2025 Results.xlsx
+++ b/TCR 2025 Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02fc7b328ab0cc43/Desktop/Github/TCR-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C81AA1E-13FD-490B-B37E-33D68D79E9CA}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B29C0B67-C1F2-4EB8-9684-7563D1E3E72C}"/>
   <bookViews>
-    <workbookView xWindow="39570" yWindow="495" windowWidth="27630" windowHeight="14880" activeTab="1" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
+    <workbookView xWindow="47895" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Record" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,89 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Gabrielle Salamanca</author>
+  </authors>
+  <commentList>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{CAB682DD-116D-41BA-B32A-6D548DDE16FC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabrielle Salamanca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+chek on this warning</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E15" authorId="0" shapeId="0" xr:uid="{91C3D906-57FA-4674-A625-0B995A115DE3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabrielle Salamanca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+too many predictors sometimes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D50" authorId="0" shapeId="0" xr:uid="{89B17D78-993D-4FA0-8A50-55100986ADFE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabrielle Salamanca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Test accuracy for consistency
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="48">
   <si>
@@ -189,7 +272,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,8 +311,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -302,6 +398,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -315,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -372,6 +474,10 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -699,11 +805,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F10ACA-FE60-4476-A75C-BE5F9F7050CA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F10ACA-FE60-4476-A75C-BE5F9F7050CA}">
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67:D74"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,7 +851,7 @@
       <c r="D2" s="2">
         <v>0.68179999999999996</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="20" t="s">
         <v>18</v>
       </c>
     </row>
@@ -757,7 +863,7 @@
       <c r="D3" s="2">
         <v>0.72729999999999995</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="21" t="s">
         <v>15</v>
       </c>
     </row>
@@ -769,7 +875,7 @@
       <c r="D4" s="2">
         <v>0.68179999999999996</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="20" t="s">
         <v>16</v>
       </c>
     </row>
@@ -906,7 +1012,7 @@
       <c r="D15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="20" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="4"/>
@@ -922,7 +1028,7 @@
       <c r="D16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="20" t="s">
         <v>19</v>
       </c>
       <c r="F16" s="4"/>
@@ -938,7 +1044,7 @@
       <c r="D17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="20" t="s">
         <v>20</v>
       </c>
       <c r="F17" s="4"/>
@@ -1737,6 +1843,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1744,8 +1851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D437B6-726D-4DC3-85CA-C3D4328315ED}">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H67" sqref="H67"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added a version 2 of the record sheet
</commit_message>
<xml_diff>
--- a/TCR 2025 Results.xlsx
+++ b/TCR 2025 Results.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02fc7b328ab0cc43/Desktop/Github/TCR-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B29C0B67-C1F2-4EB8-9684-7563D1E3E72C}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EB66A5A-22F3-4DE9-89EC-E53B7A9B44E5}"/>
   <bookViews>
-    <workbookView xWindow="47895" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="1" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Record" sheetId="1" r:id="rId1"/>
-    <sheet name="Ranking" sheetId="2" r:id="rId2"/>
+    <sheet name="Record V1" sheetId="1" r:id="rId1"/>
+    <sheet name="Record V2" sheetId="3" r:id="rId2"/>
+    <sheet name="Ranking" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -108,8 +109,66 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Gabrielle Salamanca</author>
+  </authors>
+  <commentList>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{2C1E0E32-B9EC-467D-98F6-E91EA13BF196}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabrielle Salamanca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+chek on this warning</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E15" authorId="0" shapeId="0" xr:uid="{CB4E15B8-2008-4FF9-A346-EFFBAF34F76C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabrielle Salamanca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+too many predictors sometimes</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="48">
   <si>
     <t>Method</t>
   </si>
@@ -808,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F10ACA-FE60-4476-A75C-BE5F9F7050CA}">
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1848,11 +1907,1038 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9366E5E-65E1-4F29-9C1F-DEA1ADB11B3C}">
+  <dimension ref="A1:H90"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="15" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>45949</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>45949</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.63639999999999997</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>45949</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>45949</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>45949</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
+        <v>45949</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.86360000000000003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.35"/>
+    <row r="51" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>45955</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="18">
+        <v>0.63639999999999997</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0.59089999999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0.63639999999999997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
+        <v>45952</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="2">
+        <v>0.2727</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B60" s="14"/>
+      <c r="C60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="2">
+        <v>0.2273</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B61" s="2"/>
+      <c r="C61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" s="2">
+        <v>0.2273</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B62" s="2"/>
+      <c r="C62" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" s="2">
+        <v>0.2727</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B63" s="2"/>
+      <c r="C63" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" s="2">
+        <v>0.2273</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B64" s="2"/>
+      <c r="C64" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" s="2">
+        <v>0.2273</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B65" s="2"/>
+      <c r="C65" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65" s="2">
+        <v>0.18179999999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B66" s="2"/>
+      <c r="C66" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D66" s="2">
+        <v>0.2727</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="6">
+        <v>45952</v>
+      </c>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" s="2">
+        <v>0.2273</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="2">
+        <v>0.2273</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B69" s="2"/>
+      <c r="C69" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" s="2">
+        <v>0.18179999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B70" s="2"/>
+      <c r="C70" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70" s="2">
+        <v>0.2727</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B71" s="2"/>
+      <c r="C71" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D71" s="2">
+        <v>0.2727</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B72" s="2"/>
+      <c r="C72" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D72" s="2">
+        <v>0.18179999999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B73" s="2"/>
+      <c r="C73" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D73" s="2">
+        <v>0.18179999999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B74" s="2"/>
+      <c r="C74" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D74" s="2">
+        <v>0.2727</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B75" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B76" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B77" s="2"/>
+      <c r="C77" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B78" s="2"/>
+      <c r="C78" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B79" s="2"/>
+      <c r="C79" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B80" s="2"/>
+      <c r="C80" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B81" s="2"/>
+      <c r="C81" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B82" s="2"/>
+      <c r="C82" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B83" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B84" s="14"/>
+      <c r="C84" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D84" s="2"/>
+    </row>
+    <row r="85" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B85" s="2"/>
+      <c r="C85" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" s="2"/>
+    </row>
+    <row r="86" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B86" s="2"/>
+      <c r="C86" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D86" s="2"/>
+    </row>
+    <row r="87" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B87" s="2"/>
+      <c r="C87" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D87" s="2"/>
+    </row>
+    <row r="88" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B88" s="2"/>
+      <c r="C88" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B89" s="2"/>
+      <c r="C89" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D89" s="2"/>
+    </row>
+    <row r="90" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B90" s="2"/>
+      <c r="C90" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D90" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D437B6-726D-4DC3-85CA-C3D4328315ED}">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated results of bagging
</commit_message>
<xml_diff>
--- a/TCR 2025 Results.xlsx
+++ b/TCR 2025 Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02fc7b328ab0cc43/Desktop/Github/TCR-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EB66A5A-22F3-4DE9-89EC-E53B7A9B44E5}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{382907EB-A210-4B57-859E-D9BFE734F10A}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="1" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
+    <workbookView xWindow="37125" yWindow="315" windowWidth="27630" windowHeight="14880" activeTab="1" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Record V1" sheetId="1" r:id="rId1"/>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="48">
   <si>
     <t>Method</t>
   </si>
@@ -1908,10 +1908,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9366E5E-65E1-4F29-9C1F-DEA1ADB11B3C}">
-  <dimension ref="A1:H90"/>
+  <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2652,7 +2652,7 @@
     </row>
     <row r="59" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
-        <v>45952</v>
+        <v>45955</v>
       </c>
       <c r="B59" s="15" t="s">
         <v>29</v>
@@ -2661,19 +2661,16 @@
         <v>6</v>
       </c>
       <c r="D59" s="2">
-        <v>0.2727</v>
+        <v>0.72729999999999995</v>
       </c>
     </row>
     <row r="60" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="B60" s="14"/>
       <c r="C60" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D60" s="2">
-        <v>0.2273</v>
+        <v>0.72729999999999995</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -2682,7 +2679,7 @@
         <v>8</v>
       </c>
       <c r="D61" s="2">
-        <v>0.2273</v>
+        <v>0.81820000000000004</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -2691,7 +2688,7 @@
         <v>9</v>
       </c>
       <c r="D62" s="2">
-        <v>0.2727</v>
+        <v>0.72729999999999995</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -2700,7 +2697,7 @@
         <v>10</v>
       </c>
       <c r="D63" s="2">
-        <v>0.2273</v>
+        <v>0.72729999999999995</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -2709,7 +2706,7 @@
         <v>11</v>
       </c>
       <c r="D64" s="2">
-        <v>0.2273</v>
+        <v>0.81820000000000004</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -2718,7 +2715,7 @@
         <v>12</v>
       </c>
       <c r="D65" s="2">
-        <v>0.18179999999999999</v>
+        <v>0.81820000000000004</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -2727,90 +2724,73 @@
         <v>13</v>
       </c>
       <c r="D66" s="2">
-        <v>0.2727</v>
+        <v>0.72729999999999995</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="6">
-        <v>45952</v>
-      </c>
-      <c r="B67" s="2"/>
+      <c r="B67" s="17" t="s">
+        <v>30</v>
+      </c>
       <c r="C67" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D67" s="2">
-        <v>0.2273</v>
-      </c>
+      <c r="D67" s="2"/>
     </row>
     <row r="68" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B68" s="2"/>
+      <c r="B68" s="17" t="s">
+        <v>31</v>
+      </c>
       <c r="C68" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D68" s="2">
-        <v>0.2273</v>
-      </c>
+      <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D69" s="2">
-        <v>0.18179999999999999</v>
-      </c>
+      <c r="D69" s="2"/>
     </row>
     <row r="70" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B70" s="2"/>
       <c r="C70" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D70" s="2">
-        <v>0.2727</v>
-      </c>
+      <c r="D70" s="2"/>
     </row>
     <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B71" s="2"/>
       <c r="C71" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D71" s="2">
-        <v>0.2727</v>
-      </c>
+      <c r="D71" s="2"/>
     </row>
     <row r="72" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D72" s="2">
-        <v>0.18179999999999999</v>
-      </c>
+      <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B73" s="2"/>
       <c r="C73" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D73" s="2">
-        <v>0.18179999999999999</v>
-      </c>
+      <c r="D73" s="2"/>
     </row>
     <row r="74" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D74" s="2">
-        <v>0.2727</v>
-      </c>
+      <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B75" s="17" t="s">
-        <v>30</v>
+      <c r="B75" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>6</v>
@@ -2818,9 +2798,7 @@
       <c r="D75" s="2"/>
     </row>
     <row r="76" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B76" s="17" t="s">
-        <v>31</v>
-      </c>
+      <c r="B76" s="14"/>
       <c r="C76" s="2" t="s">
         <v>7</v>
       </c>
@@ -2867,64 +2845,6 @@
         <v>13</v>
       </c>
       <c r="D82" s="2"/>
-    </row>
-    <row r="83" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B83" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D83" s="2"/>
-    </row>
-    <row r="84" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B84" s="14"/>
-      <c r="C84" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D84" s="2"/>
-    </row>
-    <row r="85" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B85" s="2"/>
-      <c r="C85" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D85" s="2"/>
-    </row>
-    <row r="86" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B86" s="2"/>
-      <c r="C86" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D86" s="2"/>
-    </row>
-    <row r="87" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B87" s="2"/>
-      <c r="C87" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D87" s="2"/>
-    </row>
-    <row r="88" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B88" s="2"/>
-      <c r="C88" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D88" s="2"/>
-    </row>
-    <row r="89" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B89" s="2"/>
-      <c r="C89" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D89" s="2"/>
-    </row>
-    <row r="90" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B90" s="2"/>
-      <c r="C90" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D90" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added random forest results
</commit_message>
<xml_diff>
--- a/TCR 2025 Results.xlsx
+++ b/TCR 2025 Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02fc7b328ab0cc43/Desktop/Github/TCR-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{382907EB-A210-4B57-859E-D9BFE734F10A}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE3028C7-7E10-4523-9179-1D76D11E09FC}"/>
   <bookViews>
-    <workbookView xWindow="37125" yWindow="315" windowWidth="27630" windowHeight="14880" activeTab="1" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="1" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Record V1" sheetId="1" r:id="rId1"/>
@@ -1911,7 +1911,7 @@
   <dimension ref="A1:H82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2734,7 +2734,9 @@
       <c r="C67" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D67" s="2"/>
+      <c r="D67" s="2">
+        <v>0.72729999999999995</v>
+      </c>
     </row>
     <row r="68" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B68" s="17" t="s">
@@ -2743,7 +2745,9 @@
       <c r="C68" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D68" s="2"/>
+      <c r="D68" s="2">
+        <v>0.72729999999999995</v>
+      </c>
     </row>
     <row r="69" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69"/>
@@ -2751,42 +2755,54 @@
       <c r="C69" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D69" s="2"/>
+      <c r="D69" s="2">
+        <v>0.81820000000000004</v>
+      </c>
     </row>
     <row r="70" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B70" s="2"/>
       <c r="C70" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D70" s="2"/>
+      <c r="D70" s="2">
+        <v>0.72729999999999995</v>
+      </c>
     </row>
     <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B71" s="2"/>
       <c r="C71" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D71" s="2"/>
+      <c r="D71" s="2">
+        <v>0.77270000000000005</v>
+      </c>
     </row>
     <row r="72" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D72" s="2"/>
+      <c r="D72" s="2">
+        <v>0.81820000000000004</v>
+      </c>
     </row>
     <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B73" s="2"/>
       <c r="C73" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D73" s="2"/>
+      <c r="D73" s="2">
+        <v>0.81820000000000004</v>
+      </c>
     </row>
     <row r="74" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D74" s="2"/>
+      <c r="D74" s="2">
+        <v>0.72729999999999995</v>
+      </c>
     </row>
     <row r="75" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B75" s="9" t="s">

</xml_diff>

<commit_message>
Added node size main loop results
</commit_message>
<xml_diff>
--- a/TCR 2025 Results.xlsx
+++ b/TCR 2025 Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02fc7b328ab0cc43/Desktop/Github/TCR-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE3028C7-7E10-4523-9179-1D76D11E09FC}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{122BC51E-0FE3-4032-B892-6889F384D437}"/>
   <bookViews>
     <workbookView xWindow="28695" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="1" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
   </bookViews>
@@ -163,12 +163,60 @@
         </r>
       </text>
     </comment>
+    <comment ref="B96" authorId="0" shapeId="0" xr:uid="{459A3BC9-C0F4-41FA-AA0E-5FC941C3FF07}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gabrielle Salamanca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+variability in this one, will record first three runs</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B104" authorId="0" shapeId="0" xr:uid="{B02260D4-3C02-43A8-9899-AF51658FC13A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gabrielle Salamanca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+variability in this one, will record first three runs</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="55">
   <si>
     <t>Method</t>
   </si>
@@ -326,12 +374,33 @@
   <si>
     <t>Bagging V2</t>
   </si>
+  <si>
+    <t>node size test</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>node size = 1</t>
+  </si>
+  <si>
+    <t>node size = 3</t>
+  </si>
+  <si>
+    <t>node size = 5</t>
+  </si>
+  <si>
+    <t>node size = 10</t>
+  </si>
+  <si>
+    <t>node size = 20</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,6 +451,35 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -476,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -537,6 +635,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1908,19 +2015,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9366E5E-65E1-4F29-9C1F-DEA1ADB11B3C}">
-  <dimension ref="A1:H82"/>
+  <dimension ref="A1:I127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B120" sqref="B120:C127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.35">
@@ -1933,14 +2042,14 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="23" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>45949</v>
       </c>
@@ -1957,7 +2066,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
         <v>7</v>
@@ -1969,7 +2078,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -1981,7 +2090,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
         <v>9</v>
@@ -1991,7 +2100,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
         <v>10</v>
@@ -2001,7 +2110,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
         <v>11</v>
@@ -2011,7 +2120,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>12</v>
@@ -2021,7 +2130,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
         <v>13</v>
@@ -2031,7 +2140,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>45949</v>
       </c>
@@ -2049,7 +2158,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
@@ -2063,7 +2172,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
@@ -2077,7 +2186,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
@@ -2091,7 +2200,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
@@ -2105,7 +2214,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
@@ -2121,7 +2230,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
@@ -2137,7 +2246,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
@@ -2153,7 +2262,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>45949</v>
       </c>
@@ -2171,7 +2280,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
@@ -2185,7 +2294,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
@@ -2199,7 +2308,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
@@ -2213,7 +2322,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
@@ -2227,7 +2336,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
@@ -2241,7 +2350,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
@@ -2255,7 +2364,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
@@ -2269,7 +2378,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>45949</v>
       </c>
@@ -2287,7 +2396,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="11" t="s">
         <v>24</v>
@@ -2303,7 +2412,7 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
@@ -2317,7 +2426,7 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
@@ -2331,7 +2440,7 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
@@ -2345,7 +2454,7 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
@@ -2359,7 +2468,7 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
@@ -2373,7 +2482,7 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
@@ -2387,7 +2496,7 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>45949</v>
       </c>
@@ -2405,7 +2514,7 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="12" t="s">
         <v>25</v>
@@ -2417,7 +2526,7 @@
         <v>0.77270000000000005</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
@@ -2427,7 +2536,7 @@
         <v>0.77270000000000005</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
@@ -2437,7 +2546,7 @@
         <v>0.77270000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
@@ -2447,7 +2556,7 @@
         <v>0.77270000000000005</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
@@ -2457,7 +2566,7 @@
         <v>0.77270000000000005</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
@@ -2467,7 +2576,7 @@
         <v>0.77270000000000005</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
@@ -2477,7 +2586,7 @@
         <v>0.77270000000000005</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>45949</v>
       </c>
@@ -2491,7 +2600,7 @@
         <v>0.72729999999999995</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="13" t="s">
         <v>26</v>
@@ -2503,7 +2612,7 @@
         <v>0.77270000000000005</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
@@ -2513,7 +2622,7 @@
         <v>0.77270000000000005</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
@@ -2523,7 +2632,7 @@
         <v>0.72729999999999995</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
@@ -2533,7 +2642,7 @@
         <v>0.72729999999999995</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
@@ -2543,7 +2652,7 @@
         <v>0.81820000000000004</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2" t="s">
@@ -2553,7 +2662,7 @@
         <v>0.81820000000000004</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
@@ -2563,8 +2672,10 @@
         <v>0.86360000000000003</v>
       </c>
     </row>
-    <row r="50" spans="1:4" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.35"/>
-    <row r="51" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="D50" s="23"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>45955</v>
       </c>
@@ -2578,7 +2689,7 @@
         <v>0.63639999999999997</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="16" t="s">
         <v>27</v>
@@ -2590,7 +2701,7 @@
         <v>0.68179999999999996</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2" t="s">
@@ -2600,7 +2711,7 @@
         <v>0.68179999999999996</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2" t="s">
@@ -2610,7 +2721,7 @@
         <v>0.72729999999999995</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
@@ -2620,7 +2731,7 @@
         <v>0.68179999999999996</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
@@ -2630,7 +2741,7 @@
         <v>0.59089999999999998</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2" t="s">
@@ -2640,7 +2751,7 @@
         <v>0.63639999999999997</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
@@ -2650,7 +2761,7 @@
         <v>0.72729999999999995</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
         <v>45955</v>
       </c>
@@ -2664,7 +2775,7 @@
         <v>0.72729999999999995</v>
       </c>
     </row>
-    <row r="60" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="14"/>
       <c r="C60" s="2" t="s">
         <v>7</v>
@@ -2673,7 +2784,7 @@
         <v>0.72729999999999995</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
       <c r="C61" s="2" t="s">
         <v>8</v>
@@ -2682,7 +2793,7 @@
         <v>0.81820000000000004</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
       <c r="C62" s="2" t="s">
         <v>9</v>
@@ -2691,7 +2802,7 @@
         <v>0.72729999999999995</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
       <c r="C63" s="2" t="s">
         <v>10</v>
@@ -2699,8 +2810,11 @@
       <c r="D63" s="2">
         <v>0.72729999999999995</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
       <c r="C64" s="2" t="s">
         <v>11</v>
@@ -2708,8 +2822,9 @@
       <c r="D64" s="2">
         <v>0.81820000000000004</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I64" s="1"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
       <c r="C65" s="2" t="s">
         <v>12</v>
@@ -2717,8 +2832,9 @@
       <c r="D65" s="2">
         <v>0.81820000000000004</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I65" s="1"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
       <c r="C66" s="2" t="s">
         <v>13</v>
@@ -2726,141 +2842,622 @@
       <c r="D66" s="2">
         <v>0.72729999999999995</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B67" s="17" t="s">
+      <c r="I66" s="1"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B67" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C67" s="1">
+        <v>1</v>
+      </c>
+      <c r="D67" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="I67" s="1"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C68" s="1">
+        <v>3</v>
+      </c>
+      <c r="D68" s="2">
+        <v>0.63639999999999997</v>
+      </c>
+      <c r="I68" s="1"/>
+    </row>
+    <row r="69" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69"/>
+      <c r="C69" s="1">
+        <v>5</v>
+      </c>
+      <c r="D69" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="F69"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C70" s="1">
+        <v>10</v>
+      </c>
+      <c r="D70" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="I70" s="1"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C71" s="1">
+        <v>20</v>
+      </c>
+      <c r="D71" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="I71" s="1"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>49</v>
+      </c>
+      <c r="B72" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C73" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C74" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C75" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D75" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C76" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D76" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C77" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D77" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C78" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D78" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C79" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D79" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B80" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C81" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C82" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C83" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D83" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C84" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D84" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C85" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D85" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C86" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D86" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C87" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D87" s="2">
+        <v>0.63639999999999997</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B88" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D88" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C89" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D89" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C90" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D90" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C91" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D91" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C92" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D92" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C93" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D93" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C94" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D94" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C95" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D95" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="24">
+        <v>45956</v>
+      </c>
+      <c r="B96" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D96" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E96" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="F96" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C97" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D97" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E97" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="F97" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C98" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D98" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E98" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="F98" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C99" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D99" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E99" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="F99" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C100" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D100" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E100" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="F100" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C101" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D101" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E101" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="F101" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C102" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D102" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E102" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="F102" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C103" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D103" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E103" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="F103" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B104" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D104" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E104" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="F104" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C105" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D105" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E105" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="F105" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C106" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D106" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E106" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="F106" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C107" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D107" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E107" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="F107" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C108" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D108" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E108" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="F108" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C109" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D109" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E109" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="F109" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C110" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D110" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E110" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="F110" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C111" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D111" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E111" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="F111" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="6">
+        <v>45955</v>
+      </c>
+      <c r="B112" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C112" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D67" s="2">
-        <v>0.72729999999999995</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B68" s="17" t="s">
+      <c r="D112" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B113" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C113" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D68" s="2">
-        <v>0.72729999999999995</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2" t="s">
+      <c r="D113" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B114" s="2"/>
+      <c r="C114" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D69" s="2">
+      <c r="D114" s="2">
         <v>0.81820000000000004</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B70" s="2"/>
-      <c r="C70" s="2" t="s">
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B115" s="2"/>
+      <c r="C115" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D70" s="2">
-        <v>0.72729999999999995</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B71" s="2"/>
-      <c r="C71" s="2" t="s">
+      <c r="D115" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B116" s="2"/>
+      <c r="C116" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D71" s="2">
-        <v>0.77270000000000005</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B72" s="2"/>
-      <c r="C72" s="2" t="s">
+      <c r="D116" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B117" s="2"/>
+      <c r="C117" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D72" s="2">
+      <c r="D117" s="2">
         <v>0.81820000000000004</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B73" s="2"/>
-      <c r="C73" s="2" t="s">
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B118" s="2"/>
+      <c r="C118" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D73" s="2">
+      <c r="D118" s="2">
         <v>0.81820000000000004</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B74" s="2"/>
-      <c r="C74" s="2" t="s">
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B119" s="2"/>
+      <c r="C119" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D74" s="2">
-        <v>0.72729999999999995</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B75" s="9" t="s">
+      <c r="D119" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B120" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C120" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D75" s="2"/>
-    </row>
-    <row r="76" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B76" s="14"/>
-      <c r="C76" s="2" t="s">
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B121" s="14"/>
+      <c r="C121" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D76" s="2"/>
-    </row>
-    <row r="77" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B77" s="2"/>
-      <c r="C77" s="2" t="s">
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B122" s="2"/>
+      <c r="C122" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D77" s="2"/>
-    </row>
-    <row r="78" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B78" s="2"/>
-      <c r="C78" s="2" t="s">
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B123" s="2"/>
+      <c r="C123" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D78" s="2"/>
-    </row>
-    <row r="79" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B79" s="2"/>
-      <c r="C79" s="2" t="s">
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B124" s="2"/>
+      <c r="C124" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D79" s="2"/>
-    </row>
-    <row r="80" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B80" s="2"/>
-      <c r="C80" s="2" t="s">
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B125" s="2"/>
+      <c r="C125" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D80" s="2"/>
-    </row>
-    <row r="81" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B81" s="2"/>
-      <c r="C81" s="2" t="s">
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B126" s="2"/>
+      <c r="C126" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D81" s="2"/>
-    </row>
-    <row r="82" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B82" s="2"/>
-      <c r="C82" s="2" t="s">
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B127" s="2"/>
+      <c r="C127" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D82" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added boosting and random forest results
</commit_message>
<xml_diff>
--- a/TCR 2025 Results.xlsx
+++ b/TCR 2025 Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02fc7b328ab0cc43/Desktop/Github/TCR-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{122BC51E-0FE3-4032-B892-6889F384D437}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5B115A7-F64B-42C7-982B-D8617E9011ED}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="1" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="15375" windowHeight="15585" activeTab="1" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Record V1" sheetId="1" r:id="rId1"/>
@@ -216,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="92">
   <si>
     <t>Method</t>
   </si>
@@ -394,6 +394,117 @@
   </si>
   <si>
     <t>node size = 20</t>
+  </si>
+  <si>
+    <t>mtry = 2</t>
+  </si>
+  <si>
+    <t>ntree = 500</t>
+  </si>
+  <si>
+    <t>mtry = 3</t>
+  </si>
+  <si>
+    <t>mtry = 4</t>
+  </si>
+  <si>
+    <t>mtry = 5</t>
+  </si>
+  <si>
+    <t>mtry = 6</t>
+  </si>
+  <si>
+    <t>best mtry = 2</t>
+  </si>
+  <si>
+    <t>OOB error = 0.2442</t>
+  </si>
+  <si>
+    <t>best mtry = 10</t>
+  </si>
+  <si>
+    <t>best mtry = 4</t>
+  </si>
+  <si>
+    <t>best mtry = 8</t>
+  </si>
+  <si>
+    <t>best mtry = 15</t>
+  </si>
+  <si>
+    <t>best mtry = 3</t>
+  </si>
+  <si>
+    <t>OOB error = 0.1628</t>
+  </si>
+  <si>
+    <t>OOB error = 0.1744</t>
+  </si>
+  <si>
+    <t>trees = 303</t>
+  </si>
+  <si>
+    <t>trees = 278</t>
+  </si>
+  <si>
+    <t>trees = 359</t>
+  </si>
+  <si>
+    <t>trees = 561</t>
+  </si>
+  <si>
+    <t>trees = 486</t>
+  </si>
+  <si>
+    <t>trees = 311</t>
+  </si>
+  <si>
+    <t>trees = 737</t>
+  </si>
+  <si>
+    <t>trees = 564</t>
+  </si>
+  <si>
+    <t>shrinkage = 0.05</t>
+  </si>
+  <si>
+    <t>depth = 4</t>
+  </si>
+  <si>
+    <t>shrinkage = 0.01</t>
+  </si>
+  <si>
+    <t>shrinkage = 0.1</t>
+  </si>
+  <si>
+    <t>depth = 2</t>
+  </si>
+  <si>
+    <t>depth = 1</t>
+  </si>
+  <si>
+    <t>trees = 59</t>
+  </si>
+  <si>
+    <t>trees = 319</t>
+  </si>
+  <si>
+    <t>trees = 79</t>
+  </si>
+  <si>
+    <t>trees = 829</t>
+  </si>
+  <si>
+    <t>trees = 62</t>
+  </si>
+  <si>
+    <t>trees = 57</t>
+  </si>
+  <si>
+    <t>trees = 968</t>
+  </si>
+  <si>
+    <t>trees = 63</t>
   </si>
 </sst>
 </file>
@@ -2015,10 +2126,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9366E5E-65E1-4F29-9C1F-DEA1ADB11B3C}">
-  <dimension ref="A1:I127"/>
+  <dimension ref="A1:I151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B120" sqref="B120:C127"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="G146" sqref="G146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2028,8 +2139,8 @@
     <col min="3" max="3" width="11.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.35">
@@ -2065,6 +2176,7 @@
       <c r="E2" s="20" t="s">
         <v>18</v>
       </c>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
@@ -2077,6 +2189,7 @@
       <c r="E3" s="21" t="s">
         <v>15</v>
       </c>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
@@ -2089,6 +2202,7 @@
       <c r="E4" s="20" t="s">
         <v>16</v>
       </c>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
@@ -2099,6 +2213,7 @@
         <v>0.81820000000000004</v>
       </c>
       <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -2109,6 +2224,7 @@
         <v>0.77270000000000005</v>
       </c>
       <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
@@ -2119,6 +2235,7 @@
         <v>0.77270000000000005</v>
       </c>
       <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
@@ -2129,6 +2246,7 @@
         <v>0.77270000000000005</v>
       </c>
       <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
@@ -2139,6 +2257,7 @@
         <v>0.77270000000000005</v>
       </c>
       <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
@@ -2154,7 +2273,7 @@
         <v>0.68179999999999996</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="4"/>
+      <c r="F10" s="2"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
@@ -2168,7 +2287,7 @@
         <v>0.72729999999999995</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="4"/>
+      <c r="F11" s="2"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
@@ -2182,7 +2301,7 @@
         <v>0.72729999999999995</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="4"/>
+      <c r="F12" s="2"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
@@ -2196,7 +2315,7 @@
         <v>0.72729999999999995</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="4"/>
+      <c r="F13" s="2"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
@@ -2210,7 +2329,7 @@
         <v>0.63639999999999997</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="4"/>
+      <c r="F14" s="2"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
@@ -2226,7 +2345,7 @@
       <c r="E15" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="4"/>
+      <c r="F15" s="2"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
@@ -2242,7 +2361,7 @@
       <c r="E16" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="4"/>
+      <c r="F16" s="2"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
@@ -2258,7 +2377,7 @@
       <c r="E17" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="4"/>
+      <c r="F17" s="2"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
@@ -2276,7 +2395,7 @@
         <v>0.68179999999999996</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="4"/>
+      <c r="F18" s="2"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
@@ -2290,7 +2409,7 @@
         <v>0.77270000000000005</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="4"/>
+      <c r="F19" s="2"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
@@ -2304,7 +2423,7 @@
         <v>0.77270000000000005</v>
       </c>
       <c r="E20" s="2"/>
-      <c r="F20" s="4"/>
+      <c r="F20" s="2"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
@@ -2318,7 +2437,7 @@
         <v>0.77270000000000005</v>
       </c>
       <c r="E21" s="2"/>
-      <c r="F21" s="4"/>
+      <c r="F21" s="2"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
@@ -2332,7 +2451,7 @@
         <v>0.81820000000000004</v>
       </c>
       <c r="E22" s="2"/>
-      <c r="F22" s="4"/>
+      <c r="F22" s="2"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
@@ -2346,7 +2465,7 @@
         <v>0.77270000000000005</v>
       </c>
       <c r="E23" s="2"/>
-      <c r="F23" s="4"/>
+      <c r="F23" s="2"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
@@ -2360,7 +2479,7 @@
         <v>0.77270000000000005</v>
       </c>
       <c r="E24" s="2"/>
-      <c r="F24" s="4"/>
+      <c r="F24" s="2"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
@@ -2374,7 +2493,7 @@
         <v>0.72729999999999995</v>
       </c>
       <c r="E25" s="2"/>
-      <c r="F25" s="4"/>
+      <c r="F25" s="2"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
@@ -2392,7 +2511,7 @@
         <v>0.72729999999999995</v>
       </c>
       <c r="E26" s="2"/>
-      <c r="F26" s="4"/>
+      <c r="F26" s="2"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
@@ -2408,7 +2527,7 @@
         <v>0.72729999999999995</v>
       </c>
       <c r="E27" s="2"/>
-      <c r="F27" s="4"/>
+      <c r="F27" s="2"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
@@ -2422,7 +2541,7 @@
         <v>0.81820000000000004</v>
       </c>
       <c r="E28" s="2"/>
-      <c r="F28" s="4"/>
+      <c r="F28" s="2"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>
@@ -2436,7 +2555,7 @@
         <v>0.77270000000000005</v>
       </c>
       <c r="E29" s="2"/>
-      <c r="F29" s="4"/>
+      <c r="F29" s="2"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
     </row>
@@ -2450,7 +2569,7 @@
         <v>0.81820000000000004</v>
       </c>
       <c r="E30" s="2"/>
-      <c r="F30" s="4"/>
+      <c r="F30" s="2"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
@@ -2464,7 +2583,7 @@
         <v>0.77270000000000005</v>
       </c>
       <c r="E31" s="2"/>
-      <c r="F31" s="4"/>
+      <c r="F31" s="2"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
     </row>
@@ -2478,7 +2597,7 @@
         <v>0.81820000000000004</v>
       </c>
       <c r="E32" s="2"/>
-      <c r="F32" s="4"/>
+      <c r="F32" s="2"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
@@ -2492,7 +2611,7 @@
         <v>0.72729999999999995</v>
       </c>
       <c r="E33" s="2"/>
-      <c r="F33" s="4"/>
+      <c r="F33" s="2"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
     </row>
@@ -2510,7 +2629,7 @@
         <v>0.72729999999999995</v>
       </c>
       <c r="E34" s="2"/>
-      <c r="F34" s="4"/>
+      <c r="F34" s="2"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
     </row>
@@ -2873,7 +2992,6 @@
       <c r="D69" s="2">
         <v>0.68179999999999996</v>
       </c>
-      <c r="F69"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C70" s="1">
@@ -3332,7 +3450,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="6">
-        <v>45955</v>
+        <v>45957</v>
       </c>
       <c r="B112" s="17" t="s">
         <v>30</v>
@@ -3343,8 +3461,11 @@
       <c r="D112" s="2">
         <v>0.72729999999999995</v>
       </c>
-    </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E112" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B113" s="17" t="s">
         <v>31</v>
       </c>
@@ -3354,17 +3475,25 @@
       <c r="D113" s="2">
         <v>0.72729999999999995</v>
       </c>
-    </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B114" s="2"/>
+      <c r="E113" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B114" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="C114" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D114" s="2">
         <v>0.81820000000000004</v>
       </c>
-    </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E114" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B115" s="2"/>
       <c r="C115" s="2" t="s">
         <v>9</v>
@@ -3372,8 +3501,11 @@
       <c r="D115" s="2">
         <v>0.72729999999999995</v>
       </c>
-    </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E115" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B116" s="2"/>
       <c r="C116" s="2" t="s">
         <v>10</v>
@@ -3381,8 +3513,11 @@
       <c r="D116" s="2">
         <v>0.77270000000000005</v>
       </c>
-    </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E116" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B117" s="2"/>
       <c r="C117" s="2" t="s">
         <v>11</v>
@@ -3390,8 +3525,11 @@
       <c r="D117" s="2">
         <v>0.81820000000000004</v>
       </c>
-    </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E117" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B118" s="2"/>
       <c r="C118" s="2" t="s">
         <v>12</v>
@@ -3399,8 +3537,11 @@
       <c r="D118" s="2">
         <v>0.81820000000000004</v>
       </c>
-    </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E118" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B119" s="2"/>
       <c r="C119" s="2" t="s">
         <v>13</v>
@@ -3408,56 +3549,411 @@
       <c r="D119" s="2">
         <v>0.72729999999999995</v>
       </c>
-    </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B120" s="9" t="s">
-        <v>32</v>
-      </c>
+      <c r="E119" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C120" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B121" s="14"/>
+      <c r="D120" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C121" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B122" s="2"/>
+      <c r="D121" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C122" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B123" s="2"/>
+      <c r="D122" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C123" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B124" s="2"/>
+      <c r="D123" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C124" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B125" s="2"/>
+      <c r="D124" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C125" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B126" s="2"/>
+      <c r="D125" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C126" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B127" s="2"/>
+      <c r="D126" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C127" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D127" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B128" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D128" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F128" s="2"/>
+      <c r="G128" s="2"/>
+    </row>
+    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B129" s="14"/>
+      <c r="C129" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D129" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F129" s="2"/>
+      <c r="G129" s="2"/>
+    </row>
+    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B130" s="2"/>
+      <c r="C130" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D130" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F130" s="2"/>
+      <c r="G130" s="2"/>
+    </row>
+    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B131" s="2"/>
+      <c r="C131" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D131" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F131" s="2"/>
+      <c r="G131" s="2"/>
+    </row>
+    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B132" s="2"/>
+      <c r="C132" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D132" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F132" s="2"/>
+      <c r="G132" s="2"/>
+    </row>
+    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B133" s="2"/>
+      <c r="C133" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D133" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F133" s="2"/>
+      <c r="G133" s="2"/>
+    </row>
+    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B134" s="2"/>
+      <c r="C134" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D134" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F134" s="2"/>
+      <c r="G134" s="2"/>
+    </row>
+    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B135" s="2"/>
+      <c r="C135" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D135" s="2">
+        <v>0.86360000000000003</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F135" s="2"/>
+      <c r="G135" s="2"/>
+    </row>
+    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C136" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D136" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G136" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C137" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D137" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G137" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C138" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D138" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G138" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C139" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D139" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G139" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C140" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D140" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G140" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C141" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D141" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G141" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C142" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D142" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G142" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C143" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D143" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G143" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="144" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E144" s="2"/>
+      <c r="F144" s="2"/>
+      <c r="G144" s="2"/>
+    </row>
+    <row r="145" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E145" s="2"/>
+      <c r="F145" s="2"/>
+      <c r="G145" s="2"/>
+    </row>
+    <row r="146" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E146" s="2"/>
+      <c r="F146" s="2"/>
+      <c r="G146" s="2"/>
+    </row>
+    <row r="147" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E147" s="2"/>
+      <c r="F147" s="2"/>
+      <c r="G147" s="2"/>
+    </row>
+    <row r="148" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E148" s="2"/>
+      <c r="F148" s="2"/>
+      <c r="G148" s="2"/>
+    </row>
+    <row r="149" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E149" s="2"/>
+      <c r="F149" s="2"/>
+      <c r="G149" s="2"/>
+    </row>
+    <row r="150" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E150" s="2"/>
+      <c r="F150" s="2"/>
+      <c r="G150" s="2"/>
+    </row>
+    <row r="151" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E151" s="2"/>
+      <c r="F151" s="2"/>
+      <c r="G151" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
spacing for the print edited; made copy of record V2, cleaned it up, and updated bagging results
</commit_message>
<xml_diff>
--- a/TCR 2025 Results.xlsx
+++ b/TCR 2025 Results.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02fc7b328ab0cc43/Desktop/Github/TCR-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5B115A7-F64B-42C7-982B-D8617E9011ED}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F8D8BCE-26BA-478C-A0D6-76CDE90C22F2}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="15375" windowHeight="15585" activeTab="1" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="2" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Record V1" sheetId="1" r:id="rId1"/>
     <sheet name="Record V2" sheetId="3" r:id="rId2"/>
-    <sheet name="Ranking" sheetId="2" r:id="rId3"/>
+    <sheet name="Record V3" sheetId="4" r:id="rId3"/>
+    <sheet name="Ranking" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -215,8 +216,66 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Gabrielle Salamanca</author>
+  </authors>
+  <commentList>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{5D8E60D0-9BB8-4649-9FBD-3008CCAB58FC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabrielle Salamanca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+chek on this warning</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E15" authorId="0" shapeId="0" xr:uid="{A764E9F2-0442-473C-B4D2-E3C3549AD83C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabrielle Salamanca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+too many predictors sometimes</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="102">
   <si>
     <t>Method</t>
   </si>
@@ -505,6 +564,36 @@
   </si>
   <si>
     <t>trees = 63</t>
+  </si>
+  <si>
+    <t>best ntree = 200</t>
+  </si>
+  <si>
+    <t>best ntree = 500</t>
+  </si>
+  <si>
+    <t>nodesize = 5</t>
+  </si>
+  <si>
+    <t>nodesize = 1</t>
+  </si>
+  <si>
+    <t>sample size = 43</t>
+  </si>
+  <si>
+    <t>sample size = 86</t>
+  </si>
+  <si>
+    <t>sample size = 60</t>
+  </si>
+  <si>
+    <t>OOB error = 0.2326</t>
+  </si>
+  <si>
+    <t>OOB error = 0.1512</t>
+  </si>
+  <si>
+    <t>OOB error = 0.1860</t>
   </si>
 </sst>
 </file>
@@ -2128,8 +2217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9366E5E-65E1-4F29-9C1F-DEA1ADB11B3C}">
   <dimension ref="A1:I151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="G146" sqref="G146"/>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3963,10 +4052,1526 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F193E77-64AE-427B-86BC-A5B421AD438C}">
+  <dimension ref="A1:H151"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="H73" sqref="H73"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="15" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>45949</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>45949</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.63639999999999997</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>45949</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>45949</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>45949</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
+        <v>45949</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.86360000000000003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="D50" s="23"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>45955</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="18">
+        <v>0.63639999999999997</v>
+      </c>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0.59089999999999998</v>
+      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0.63639999999999997</v>
+      </c>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
+        <v>45968</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="4"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D66" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="6">
+        <v>45957</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="4"/>
+      <c r="B68" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+    </row>
+    <row r="69" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="4"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="4"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D71" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="4"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D72" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="4"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D73" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="4"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D74" s="2">
+        <v>0.86360000000000003</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="4"/>
+      <c r="B75" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H75" s="2"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="4"/>
+      <c r="B76" s="14"/>
+      <c r="C76" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H76" s="2"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="4"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H77" s="2"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="4"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D78" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H78" s="2"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="4"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D79" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H79" s="2"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="4"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D80" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H80" s="2"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="4"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D81" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H81" s="2"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="4"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D82" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H82" s="2"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="F83"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="F84"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+      <c r="F85"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
+      <c r="F86"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="F87"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
+      <c r="F88"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="F89"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
+      <c r="F90"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
+      <c r="F91"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
+      <c r="F92"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+      <c r="F93"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B94" s="2"/>
+      <c r="C94" s="2"/>
+      <c r="F94"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
+      <c r="F95"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="24"/>
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+      <c r="E96"/>
+      <c r="F96"/>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B97" s="2"/>
+      <c r="C97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97"/>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B98" s="2"/>
+      <c r="C98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98"/>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B99" s="2"/>
+      <c r="C99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99"/>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B100" s="2"/>
+      <c r="C100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100"/>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101"/>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102"/>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B103" s="2"/>
+      <c r="C103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103"/>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B104" s="2"/>
+      <c r="C104" s="2"/>
+      <c r="E104" s="2"/>
+      <c r="F104"/>
+    </row>
+    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B105" s="2"/>
+      <c r="C105" s="2"/>
+      <c r="E105" s="2"/>
+      <c r="F105"/>
+    </row>
+    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B106" s="2"/>
+      <c r="C106" s="2"/>
+      <c r="E106" s="2"/>
+      <c r="F106"/>
+    </row>
+    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C107" s="2"/>
+      <c r="E107" s="2"/>
+      <c r="F107" s="2"/>
+    </row>
+    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C108" s="2"/>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
+    </row>
+    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C109" s="2"/>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C110" s="2"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2"/>
+    </row>
+    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C111" s="2"/>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2"/>
+    </row>
+    <row r="136" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E136" s="2"/>
+    </row>
+    <row r="137" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E137" s="2"/>
+    </row>
+    <row r="138" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E138" s="2"/>
+    </row>
+    <row r="139" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E139" s="2"/>
+    </row>
+    <row r="140" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E140" s="2"/>
+    </row>
+    <row r="141" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E141" s="2"/>
+    </row>
+    <row r="142" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E142" s="2"/>
+    </row>
+    <row r="143" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E143" s="2"/>
+    </row>
+    <row r="144" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F144" s="2"/>
+      <c r="G144" s="2"/>
+    </row>
+    <row r="145" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F145" s="2"/>
+      <c r="G145" s="2"/>
+    </row>
+    <row r="146" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F146" s="2"/>
+      <c r="G146" s="2"/>
+    </row>
+    <row r="147" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F147" s="2"/>
+      <c r="G147" s="2"/>
+    </row>
+    <row r="148" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F148" s="2"/>
+      <c r="G148" s="2"/>
+    </row>
+    <row r="149" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F149" s="2"/>
+      <c r="G149" s="2"/>
+    </row>
+    <row r="150" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F150" s="2"/>
+      <c r="G150" s="2"/>
+    </row>
+    <row r="151" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F151" s="2"/>
+      <c r="G151" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D437B6-726D-4DC3-85CA-C3D4328315ED}">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="A50" sqref="A50:XFD50"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated boosting and random forest, rid of V2 values
</commit_message>
<xml_diff>
--- a/TCR 2025 Results.xlsx
+++ b/TCR 2025 Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02fc7b328ab0cc43/Desktop/Github/TCR-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F8D8BCE-26BA-478C-A0D6-76CDE90C22F2}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EECE3E9-9FD0-4715-909C-A009422C2F85}"/>
   <bookViews>
     <workbookView xWindow="28695" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="2" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
   </bookViews>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="131">
   <si>
     <t>Method</t>
   </si>
@@ -594,6 +594,93 @@
   </si>
   <si>
     <t>OOB error = 0.1860</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cumulative </t>
+  </si>
+  <si>
+    <t>Attempt</t>
+  </si>
+  <si>
+    <t>best ntree = 1</t>
+  </si>
+  <si>
+    <t>best ntree = 38</t>
+  </si>
+  <si>
+    <t>best ntree = 289</t>
+  </si>
+  <si>
+    <t>best ntree = 131</t>
+  </si>
+  <si>
+    <t>best ntree = 82</t>
+  </si>
+  <si>
+    <t>best ntree = 161</t>
+  </si>
+  <si>
+    <t>best ntree = 78</t>
+  </si>
+  <si>
+    <t>best ntree = 31</t>
+  </si>
+  <si>
+    <t>nodesize = 2</t>
+  </si>
+  <si>
+    <t>nodesize = 9</t>
+  </si>
+  <si>
+    <t>sample size = 64</t>
+  </si>
+  <si>
+    <t>sample size = 52</t>
+  </si>
+  <si>
+    <t>sample size = 77</t>
+  </si>
+  <si>
+    <t>OOB error = 0.1667</t>
+  </si>
+  <si>
+    <t>OOB error = 0.1279</t>
+  </si>
+  <si>
+    <t>OOB error = 0.1395</t>
+  </si>
+  <si>
+    <t>best mtry = 5</t>
+  </si>
+  <si>
+    <t>best mtry = 9</t>
+  </si>
+  <si>
+    <t>best mtry = 6</t>
+  </si>
+  <si>
+    <t>depth = 3</t>
+  </si>
+  <si>
+    <t>trees = 18</t>
+  </si>
+  <si>
+    <t>trees = 388</t>
+  </si>
+  <si>
+    <t>trees = 477</t>
+  </si>
+  <si>
+    <t>trees = 47</t>
+  </si>
+  <si>
+    <t>trees = 192</t>
+  </si>
+  <si>
+    <t>trees = 166</t>
+  </si>
+  <si>
+    <t>trees = 992</t>
   </si>
 </sst>
 </file>
@@ -2217,7 +2304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9366E5E-65E1-4F29-9C1F-DEA1ADB11B3C}">
   <dimension ref="A1:I151"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
+    <sheetView topLeftCell="A117" workbookViewId="0">
       <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
@@ -4055,14 +4142,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F193E77-64AE-427B-86BC-A5B421AD438C}">
   <dimension ref="A1:H151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="H73" sqref="H73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="15" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" style="1" customWidth="1"/>
@@ -4223,7 +4310,6 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
@@ -4237,7 +4323,6 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
@@ -4251,7 +4336,6 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
         <v>9</v>
       </c>
@@ -4265,7 +4349,6 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
         <v>10</v>
       </c>
@@ -4279,7 +4362,6 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
         <v>11</v>
       </c>
@@ -4295,7 +4377,6 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
         <v>12</v>
       </c>
@@ -4311,7 +4392,6 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
         <v>13</v>
       </c>
@@ -4345,7 +4425,6 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
-      <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
         <v>7</v>
       </c>
@@ -4359,7 +4438,6 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
         <v>8</v>
       </c>
@@ -4373,7 +4451,6 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-      <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
         <v>9</v>
       </c>
@@ -4387,7 +4464,6 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
         <v>10</v>
       </c>
@@ -4401,7 +4477,6 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-      <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
         <v>11</v>
       </c>
@@ -4415,7 +4490,6 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
         <v>12</v>
       </c>
@@ -4429,7 +4503,6 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
         <v>13</v>
       </c>
@@ -4477,7 +4550,6 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
         <v>8</v>
       </c>
@@ -4491,7 +4563,6 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
         <v>9</v>
       </c>
@@ -4505,7 +4576,6 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
-      <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
         <v>10</v>
       </c>
@@ -4519,7 +4589,6 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
-      <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
         <v>11</v>
       </c>
@@ -4533,7 +4602,6 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
-      <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
         <v>12</v>
       </c>
@@ -4547,7 +4615,6 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
-      <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
         <v>13</v>
       </c>
@@ -4591,7 +4658,6 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
-      <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
         <v>8</v>
       </c>
@@ -4601,7 +4667,6 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
-      <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
         <v>9</v>
       </c>
@@ -4611,7 +4676,6 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
-      <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
         <v>10</v>
       </c>
@@ -4621,7 +4685,6 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
-      <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
         <v>11</v>
       </c>
@@ -4631,7 +4694,6 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
-      <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
         <v>12</v>
       </c>
@@ -4641,7 +4703,6 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
-      <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
         <v>13</v>
       </c>
@@ -4677,7 +4738,6 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
-      <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
         <v>8</v>
       </c>
@@ -4687,7 +4747,6 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
-      <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
         <v>9</v>
       </c>
@@ -4697,7 +4756,6 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
-      <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
         <v>10</v>
       </c>
@@ -4707,7 +4765,6 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
-      <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
         <v>11</v>
       </c>
@@ -4717,7 +4774,6 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
-      <c r="B48" s="2"/>
       <c r="C48" s="2" t="s">
         <v>12</v>
       </c>
@@ -4727,7 +4783,6 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
-      <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
         <v>13</v>
       </c>
@@ -4736,6 +4791,7 @@
       </c>
     </row>
     <row r="50" spans="1:8" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B50" s="23"/>
       <c r="D50" s="23"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -4773,7 +4829,6 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
-      <c r="B53" s="2"/>
       <c r="C53" s="2" t="s">
         <v>8</v>
       </c>
@@ -4787,7 +4842,6 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
-      <c r="B54" s="2"/>
       <c r="C54" s="2" t="s">
         <v>9</v>
       </c>
@@ -4801,7 +4855,6 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
-      <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
         <v>10</v>
       </c>
@@ -4815,7 +4868,6 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
-      <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
         <v>11</v>
       </c>
@@ -4829,7 +4881,6 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
-      <c r="B57" s="2"/>
       <c r="C57" s="2" t="s">
         <v>12</v>
       </c>
@@ -4843,7 +4894,6 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
-      <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
         <v>13</v>
       </c>
@@ -4905,7 +4955,6 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
-      <c r="B61" s="2"/>
       <c r="C61" s="2" t="s">
         <v>8</v>
       </c>
@@ -4927,7 +4976,6 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
-      <c r="B62" s="2"/>
       <c r="C62" s="2" t="s">
         <v>9</v>
       </c>
@@ -4949,7 +4997,6 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
-      <c r="B63" s="2"/>
       <c r="C63" s="2" t="s">
         <v>10</v>
       </c>
@@ -4971,7 +5018,6 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
-      <c r="B64" s="2"/>
       <c r="C64" s="2" t="s">
         <v>11</v>
       </c>
@@ -4993,7 +5039,6 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
-      <c r="B65" s="2"/>
       <c r="C65" s="2" t="s">
         <v>12</v>
       </c>
@@ -5015,7 +5060,6 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
-      <c r="B66" s="2"/>
       <c r="C66" s="2" t="s">
         <v>13</v>
       </c>
@@ -5036,46 +5080,51 @@
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="6">
-        <v>45957</v>
-      </c>
-      <c r="B67" s="17" t="s">
-        <v>30</v>
+      <c r="B67" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D67" s="2">
-        <v>0.68179999999999996</v>
+        <v>0.72729999999999995</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
+        <v>112</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
-      <c r="B68" s="17" t="s">
-        <v>31</v>
+      <c r="B68" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D68" s="2">
-        <v>0.77270000000000005</v>
+        <v>0.72729999999999995</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
+        <v>95</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="69" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
@@ -5084,38 +5133,44 @@
         <v>8</v>
       </c>
       <c r="D69" s="2">
-        <v>0.81820000000000004</v>
+        <v>0.72729999999999995</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
+        <v>95</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
-      <c r="B70" s="2"/>
       <c r="C70" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D70" s="2">
-        <v>0.72729999999999995</v>
+        <v>0.77270000000000005</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
+        <v>95</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
-      <c r="B71" s="2"/>
       <c r="C71" s="2" t="s">
         <v>10</v>
       </c>
@@ -5123,17 +5178,20 @@
         <v>0.72729999999999995</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G71" s="2"/>
-      <c r="H71" s="2"/>
+        <v>95</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
-      <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
         <v>11</v>
       </c>
@@ -5141,95 +5199,102 @@
         <v>0.81820000000000004</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G72" s="2"/>
-      <c r="H72" s="2"/>
+        <v>95</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
-      <c r="B73" s="2"/>
       <c r="C73" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D73" s="2">
-        <v>0.81820000000000004</v>
+        <v>0.77270000000000005</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
+        <v>113</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
-      <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D74" s="2">
-        <v>0.86360000000000003</v>
+        <v>0.63639999999999997</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>77</v>
+        <v>111</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
+        <v>112</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="4"/>
-      <c r="B75" s="9" t="s">
-        <v>32</v>
+      <c r="A75" s="6">
+        <v>45968</v>
+      </c>
+      <c r="B75" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D75" s="2">
-        <v>0.68179999999999996</v>
+        <v>0.72729999999999995</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G75" s="2" t="s">
-        <v>84</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="4"/>
-      <c r="B76" s="14"/>
+      <c r="B76" s="17" t="s">
+        <v>31</v>
+      </c>
       <c r="C76" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D76" s="2">
-        <v>0.77270000000000005</v>
+        <v>0.72729999999999995</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G76" s="2" t="s">
-        <v>85</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="4"/>
-      <c r="B77" s="2"/>
       <c r="C77" s="2" t="s">
         <v>8</v>
       </c>
@@ -5237,39 +5302,31 @@
         <v>0.81820000000000004</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>78</v>
+        <v>120</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G77" s="2" t="s">
-        <v>86</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-      <c r="B78" s="2"/>
       <c r="C78" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D78" s="2">
-        <v>0.72729999999999995</v>
+        <v>0.77270000000000005</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G78" s="2" t="s">
-        <v>87</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
-      <c r="B79" s="2"/>
       <c r="C79" s="2" t="s">
         <v>10</v>
       </c>
@@ -5277,19 +5334,15 @@
         <v>0.81820000000000004</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G79" s="2" t="s">
-        <v>88</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="4"/>
-      <c r="B80" s="2"/>
       <c r="C80" s="2" t="s">
         <v>11</v>
       </c>
@@ -5297,19 +5350,15 @@
         <v>0.81820000000000004</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G80" s="2" t="s">
-        <v>89</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
-      <c r="B81" s="2"/>
       <c r="C81" s="2" t="s">
         <v>12</v>
       </c>
@@ -5317,189 +5366,230 @@
         <v>0.81820000000000004</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>90</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
-      <c r="B82" s="2"/>
       <c r="C82" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D82" s="2">
-        <v>0.77270000000000005</v>
+        <v>0.81820000000000004</v>
       </c>
       <c r="E82" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G82" s="2"/>
+      <c r="H82" s="2"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B83" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D83" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E83" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F82" s="2" t="s">
+      <c r="F83" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H83"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B84" s="14"/>
+      <c r="C84" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D84" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H84"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C85" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H85"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="24"/>
+      <c r="C86" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D86" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H86"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C87" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D87" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F87" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G82" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H82" s="2"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-      <c r="F83"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
-      <c r="F84"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="F85"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
-      <c r="F86"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
-      <c r="F87"/>
+      <c r="G87" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H87"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
-      <c r="F88"/>
+      <c r="C88" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D88" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H88"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
-      <c r="F89"/>
+      <c r="C89" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D89" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H89"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B90" s="2"/>
-      <c r="C90" s="2"/>
-      <c r="F90"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B91" s="2"/>
-      <c r="C91" s="2"/>
-      <c r="F91"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
-      <c r="F92"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
-      <c r="F93"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B94" s="2"/>
-      <c r="C94" s="2"/>
-      <c r="F94"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B95" s="2"/>
-      <c r="C95" s="2"/>
-      <c r="F95"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="24"/>
-      <c r="B96" s="2"/>
-      <c r="C96" s="2"/>
-      <c r="E96"/>
-      <c r="F96"/>
-    </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
-      <c r="E97" s="2"/>
-      <c r="F97"/>
-    </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
-      <c r="E98" s="2"/>
-      <c r="F98"/>
-    </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
-      <c r="E99" s="2"/>
-      <c r="F99"/>
-    </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
-      <c r="E100" s="2"/>
-      <c r="F100"/>
-    </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B101" s="2"/>
+      <c r="C90" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D90" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="H90"/>
+    </row>
+    <row r="101" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C101" s="2"/>
       <c r="E101" s="2"/>
       <c r="F101"/>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B102" s="2"/>
+    <row r="102" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C102" s="2"/>
       <c r="E102" s="2"/>
       <c r="F102"/>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B103" s="2"/>
+    <row r="103" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C103" s="2"/>
       <c r="E103" s="2"/>
       <c r="F103"/>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B104" s="2"/>
+    <row r="104" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C104" s="2"/>
       <c r="E104" s="2"/>
       <c r="F104"/>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B105" s="2"/>
+    <row r="105" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105"/>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B106" s="2"/>
+    <row r="106" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C106" s="2"/>
       <c r="E106" s="2"/>
       <c r="F106"/>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C107" s="2"/>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C108" s="2"/>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C109" s="2"/>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C110" s="2"/>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>

</xml_diff>

<commit_message>
Added notes abt Bagging and random forest
</commit_message>
<xml_diff>
--- a/TCR 2025 Results.xlsx
+++ b/TCR 2025 Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02fc7b328ab0cc43/Desktop/Github/TCR-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EECE3E9-9FD0-4715-909C-A009422C2F85}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E0DCA8A-7315-4A1B-9A66-3CBDC6C2F33A}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="2" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
+    <workbookView xWindow="47895" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="2" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Record V1" sheetId="1" r:id="rId1"/>
@@ -267,6 +267,54 @@
           </rPr>
           <t xml:space="preserve">
 too many predictors sometimes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B59" authorId="0" shapeId="0" xr:uid="{6949903E-7BC8-46AF-8731-FA85D50CA961}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabrielle Salamanca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+special case of random forest, consider removing</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G59" authorId="0" shapeId="0" xr:uid="{C0847C85-7A81-4085-AF4D-60C77894E59B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabrielle Salamanca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+no need for sample size</t>
         </r>
       </text>
     </comment>
@@ -2304,7 +2352,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9366E5E-65E1-4F29-9C1F-DEA1ADB11B3C}">
   <dimension ref="A1:I151"/>
   <sheetViews>
-    <sheetView topLeftCell="A117" workbookViewId="0">
+    <sheetView topLeftCell="A114" workbookViewId="0">
       <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
@@ -4142,8 +4190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F193E77-64AE-427B-86BC-A5B421AD438C}">
   <dimension ref="A1:H151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
New record sheet and updated the advanced techniques Test Accuracies
</commit_message>
<xml_diff>
--- a/TCR 2025 Results.xlsx
+++ b/TCR 2025 Results.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02fc7b328ab0cc43/Desktop/Github/TCR-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E0DCA8A-7315-4A1B-9A66-3CBDC6C2F33A}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="8_{63766BF1-CE01-4EBE-9D38-647C6EEA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{956299A3-2064-478D-905E-1D1B3631F555}"/>
   <bookViews>
-    <workbookView xWindow="47895" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="2" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="3" xr2:uid="{533619AA-80D1-4C98-AAEC-AF44897767DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Record V1" sheetId="1" r:id="rId1"/>
     <sheet name="Record V2" sheetId="3" r:id="rId2"/>
     <sheet name="Record V3" sheetId="4" r:id="rId3"/>
-    <sheet name="Ranking" sheetId="2" r:id="rId4"/>
+    <sheet name="Record V4" sheetId="5" r:id="rId4"/>
+    <sheet name="Ranking" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -322,8 +323,66 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Gabrielle Salamanca</author>
+  </authors>
+  <commentList>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{80FED8A4-E928-4A4A-9934-D116F48607AF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabrielle Salamanca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+chek on this warning</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E15" authorId="0" shapeId="0" xr:uid="{5938A46C-FA49-4424-A677-46D0EB884EA9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabrielle Salamanca:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+too many predictors sometimes</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="139">
   <si>
     <t>Method</t>
   </si>
@@ -729,6 +788,30 @@
   </si>
   <si>
     <t>trees = 992</t>
+  </si>
+  <si>
+    <t>best mtry = 30</t>
+  </si>
+  <si>
+    <t>trees = 352</t>
+  </si>
+  <si>
+    <t>trees = 29</t>
+  </si>
+  <si>
+    <t>trees = 152</t>
+  </si>
+  <si>
+    <t>trees = 942</t>
+  </si>
+  <si>
+    <t>trees = 147</t>
+  </si>
+  <si>
+    <t>trees = 94</t>
+  </si>
+  <si>
+    <t>trees = 1358</t>
   </si>
 </sst>
 </file>
@@ -4190,7 +4273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F193E77-64AE-427B-86BC-A5B421AD438C}">
   <dimension ref="A1:H151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -5706,6 +5789,1256 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C447F053-1CB7-427A-8CBC-064B37808365}">
+  <dimension ref="A1:H135"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="15" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>45949</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>45949</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="C14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.63639999999999997</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="C15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="C16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="C17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>45949</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="C19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="C20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="C21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="C22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="C23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="C24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="C25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>45949</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="C28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="C29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="C30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="C31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="C32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="C33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>45949</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="C36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="C37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="C38" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="C39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="C40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="C41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
+        <v>45949</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="C44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="C45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="C46" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="C47" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="C48" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="C49" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.86360000000000003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B50" s="23"/>
+      <c r="D50" s="23"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>45972</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="18">
+        <v>0.63639999999999997</v>
+      </c>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="C53" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="C54" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="C55" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="C56" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0.59089999999999998</v>
+      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="C57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0.63639999999999997</v>
+      </c>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="C58" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="6"/>
+      <c r="B59" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C62" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C63" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C64" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C65" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C66" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D66" s="2">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H67"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="14"/>
+      <c r="C68" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="2">
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H68"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C69" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H69"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="24"/>
+      <c r="C70" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H70"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C71" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D71" s="2">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H71"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C72" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D72" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H72"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C73" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D73" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H73"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C74" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D74" s="2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H74"/>
+    </row>
+    <row r="85" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85"/>
+    </row>
+    <row r="86" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86"/>
+    </row>
+    <row r="87" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87"/>
+    </row>
+    <row r="88" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88"/>
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88"/>
+    </row>
+    <row r="89" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89"/>
+    </row>
+    <row r="90" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90"/>
+    </row>
+    <row r="91" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+    </row>
+    <row r="92" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92"/>
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+    </row>
+    <row r="93" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+    </row>
+    <row r="94" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94"/>
+      <c r="B94" s="2"/>
+      <c r="C94" s="2"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+    </row>
+    <row r="95" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+    </row>
+    <row r="120" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120"/>
+      <c r="B120" s="2"/>
+      <c r="D120" s="2"/>
+      <c r="E120" s="2"/>
+    </row>
+    <row r="121" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121"/>
+      <c r="B121" s="2"/>
+      <c r="D121" s="2"/>
+      <c r="E121" s="2"/>
+    </row>
+    <row r="122" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122"/>
+      <c r="B122" s="2"/>
+      <c r="D122" s="2"/>
+      <c r="E122" s="2"/>
+    </row>
+    <row r="123" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123"/>
+      <c r="B123" s="2"/>
+      <c r="D123" s="2"/>
+      <c r="E123" s="2"/>
+    </row>
+    <row r="124" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124"/>
+      <c r="B124" s="2"/>
+      <c r="D124" s="2"/>
+      <c r="E124" s="2"/>
+    </row>
+    <row r="125" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125"/>
+      <c r="B125" s="2"/>
+      <c r="D125" s="2"/>
+      <c r="E125" s="2"/>
+    </row>
+    <row r="126" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126"/>
+      <c r="B126" s="2"/>
+      <c r="D126" s="2"/>
+      <c r="E126" s="2"/>
+    </row>
+    <row r="127" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127"/>
+      <c r="B127" s="2"/>
+      <c r="D127" s="2"/>
+      <c r="E127" s="2"/>
+    </row>
+    <row r="128" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128"/>
+      <c r="B128" s="2"/>
+      <c r="D128" s="2"/>
+      <c r="F128" s="2"/>
+      <c r="G128" s="2"/>
+    </row>
+    <row r="129" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129"/>
+      <c r="B129" s="2"/>
+      <c r="D129" s="2"/>
+      <c r="F129" s="2"/>
+      <c r="G129" s="2"/>
+    </row>
+    <row r="130" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130"/>
+      <c r="B130" s="2"/>
+      <c r="D130" s="2"/>
+      <c r="F130" s="2"/>
+      <c r="G130" s="2"/>
+    </row>
+    <row r="131" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131"/>
+      <c r="B131" s="2"/>
+      <c r="D131" s="2"/>
+      <c r="F131" s="2"/>
+      <c r="G131" s="2"/>
+    </row>
+    <row r="132" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132"/>
+      <c r="B132" s="2"/>
+      <c r="D132" s="2"/>
+      <c r="F132" s="2"/>
+      <c r="G132" s="2"/>
+    </row>
+    <row r="133" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133"/>
+      <c r="B133" s="2"/>
+      <c r="D133" s="2"/>
+      <c r="F133" s="2"/>
+      <c r="G133" s="2"/>
+    </row>
+    <row r="134" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134"/>
+      <c r="B134" s="2"/>
+      <c r="D134" s="2"/>
+      <c r="F134" s="2"/>
+      <c r="G134" s="2"/>
+    </row>
+    <row r="135" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135"/>
+      <c r="B135" s="2"/>
+      <c r="D135" s="2"/>
+      <c r="F135" s="2"/>
+      <c r="G135" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D437B6-726D-4DC3-85CA-C3D4328315ED}">
   <dimension ref="A1:J90"/>
   <sheetViews>

</xml_diff>